<commit_message>
fix for GitHub pages
</commit_message>
<xml_diff>
--- a/tetris-4k-archive.xlsx
+++ b/tetris-4k-archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493d989091475df7/Personal/GitHub/tetris4karchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73B61696-910D-C645-AD37-B5C32EB9D4DF}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFF2FAF8-6171-9E4A-976A-67888B1337A1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21120" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Gravity</t>
   </si>
   <si>
-    <t>https://github.com/pellsson/tinytris</t>
-  </si>
-  <si>
     <t>Pellsson</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Music</t>
   </si>
   <si>
-    <t>https://board.flatassembler.net/topic.php?p=211564#211831</t>
-  </si>
-  <si>
     <t>Arek Michowski</t>
   </si>
   <si>
@@ -188,12 +182,6 @@
     <t>Andrew March</t>
   </si>
   <si>
-    <t>https://codegolf.stackexchange.com/a/121622/120787</t>
-  </si>
-  <si>
-    <t>https://github.com/veu/mini-tetris</t>
-  </si>
-  <si>
     <t>http://www.p01.org/256b_tetris_theme</t>
   </si>
   <si>
@@ -389,7 +377,19 @@
     <t>Bytes per feature</t>
   </si>
   <si>
-    <t>https://gist.github.com/aemkei/1672254</t>
+    <t>https://nineteendo.github.io/tetris4karchive/binary-tetris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetros105</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/mini-tetris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/binary-tetris-2</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tinytris</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:R1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,46 +946,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>12</v>
@@ -994,34 +994,34 @@
         <v>10</v>
       </c>
       <c r="R1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="X1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="V1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="AB1" s="9" t="s">
         <v>9</v>
@@ -1030,88 +1030,88 @@
         <v>11</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AE1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AM1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AO1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AS1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AO1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AT1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AU1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AV1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AX1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AT1" s="9" t="s">
+      <c r="AY1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AV1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW1" s="9" t="s">
+      <c r="BA1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AX1" s="9" t="s">
+      <c r="BB1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="BD1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="BE1" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="BA1" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC1" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="BD1" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="BE1" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="BF1" s="2"/>
     </row>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="3" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1357,19 +1357,19 @@
         <v>1</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="7" t="b">
         <v>0</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="4" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>7</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="5" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -1709,19 +1709,19 @@
         <v>1</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="7" t="b">
         <v>1</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="6" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -1885,19 +1885,19 @@
         <v>0</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="7" t="b">
         <v>0</v>
@@ -2025,12 +2025,12 @@
         <v>34.25</v>
       </c>
     </row>
-    <row r="7" spans="1:58" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="8" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
@@ -2382,7 +2382,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>7</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="10" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>2</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="11" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
@@ -2907,10 +2907,10 @@
     </row>
     <row r="12" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>7</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="13" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
@@ -3117,19 +3117,19 @@
         <v>0</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M13" s="7" t="b">
         <v>0</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O13" s="7" t="b">
         <v>0</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="7" t="b">
         <v>0</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="14" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>7</v>
@@ -3435,13 +3435,13 @@
     </row>
     <row r="15" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6">
         <v>457</v>
@@ -3475,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O15" s="7" t="b">
         <v>1</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="16" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>13</v>
@@ -3645,19 +3645,19 @@
         <v>1</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="7" t="b">
         <v>1</v>
@@ -3787,10 +3787,10 @@
     </row>
     <row r="17" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
@@ -3963,10 +3963,10 @@
     </row>
     <row r="18" spans="1:57" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>7</v>
@@ -4139,10 +4139,10 @@
     </row>
     <row r="19" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -4173,19 +4173,19 @@
         <v>1</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M19" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O19" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="7" t="b">
         <v>1</v>
@@ -4315,10 +4315,10 @@
     </row>
     <row r="20" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -4352,16 +4352,16 @@
         <v>1</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O20" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q20" s="7" t="b">
         <v>1</v>
@@ -4491,10 +4491,10 @@
     </row>
     <row r="21" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
@@ -4667,13 +4667,13 @@
     </row>
     <row r="22" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="6">
         <v>2738</v>
@@ -4707,7 +4707,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O22" s="7" t="b">
         <v>0</v>
@@ -4843,13 +4843,13 @@
     </row>
     <row r="23" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D23" s="6">
         <v>3998</v>
@@ -4877,13 +4877,13 @@
         <v>1</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O23" s="7" t="b">
         <v>1</v>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>5</v>
@@ -5195,10 +5195,10 @@
     </row>
     <row r="25" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>4</v>
@@ -5229,19 +5229,19 @@
         <v>1</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O25" s="7" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q25" s="7" t="b">
         <v>1</v>
@@ -5371,13 +5371,13 @@
     </row>
     <row r="26" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D26" s="6">
         <v>4095</v>
@@ -5405,13 +5405,13 @@
         <v>1</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M26" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O26" s="7" t="b">
         <v>0</v>
@@ -5547,13 +5547,13 @@
     </row>
     <row r="27" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D27" s="6">
         <v>2882</v>
@@ -5581,13 +5581,13 @@
         <v>1</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M27" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O27" s="7" t="b">
         <v>0</v>
@@ -5723,13 +5723,13 @@
     </row>
     <row r="28" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D28" s="6">
         <v>4002</v>
@@ -5763,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O28" s="7" t="b">
         <v>1</v>
@@ -5971,7 +5971,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" location="211831" xr:uid="{76EB020E-CC71-B148-9424-BB7A1349A5E9}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{76EB020E-CC71-B148-9424-BB7A1349A5E9}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{022DC04F-D95A-7246-8451-7C3BA522CD1C}"/>
     <hyperlink ref="A9" r:id="rId3" xr:uid="{2766802B-21EA-A840-BA76-FAB4AC15193F}"/>
     <hyperlink ref="A12" r:id="rId4" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>

</xml_diff>

<commit_message>
more lists in overview
</commit_message>
<xml_diff>
--- a/tetris-4k-archive.xlsx
+++ b/tetris-4k-archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493d989091475df7/Personal/GitHub/tetris4karchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96FA9B2F-E718-4E41-9853-F1A38531CF25}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A62669B1-C19F-9847-86C3-43CD01DF2B45}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21140" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,22 +536,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -923,7 +923,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,11 +1141,11 @@
         <v>23</v>
       </c>
       <c r="K2" s="6">
-        <f>COUNTIF(K$3:K$28, "SYS")+COUNTIF(K$3:K$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="L2" s="6">
-        <f>COUNTIF(L$3:L$28, "SYS")+COUNTIF(L$3:L$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="M2" s="6">
@@ -1153,67 +1153,67 @@
         <v>16</v>
       </c>
       <c r="N2" s="6">
-        <f>COUNTIF(N$3:N$28, "SYS")+COUNTIF(N$3:N$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="O2" s="6">
-        <f>COUNTIF(O$3:O$28, "SYS")+COUNTIF(O$3:O$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="P2" s="6">
-        <f t="shared" ref="P2:AC2" si="1">COUNTIF(P$3:P$28, "SYS")+COUNTIF(P$3:P$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="Q2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="R2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="S2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="T2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="U2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="V2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="W2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="X2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Z2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="AA2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="AB2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AC2" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AD2" s="6">
@@ -1225,11 +1225,11 @@
         <v>5</v>
       </c>
       <c r="AF2" s="6">
-        <f>COUNTIF(AF$3:AF$28, "SYS")+COUNTIF(AF$3:AF$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AG2" s="6">
-        <f>COUNTIF(AG$3:AG$28, "SYS")+COUNTIF(AG$3:AG$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AH2" s="6">
@@ -1265,15 +1265,15 @@
         <v>3</v>
       </c>
       <c r="AP2" s="6">
-        <f>COUNTIF(AP$3:AP$28, "SYS")+COUNTIF(AP$3:AP$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AQ2" s="6">
-        <f>COUNTIF(AQ$3:AQ$28, "SYS")+COUNTIF(AQ$3:AQ$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR2" s="6">
-        <f>COUNTIF(AR$3:AR$28, "SYS")+COUNTIF(AR$3:AR$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS2" s="6">
@@ -1305,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="AZ2" s="6">
-        <f>COUNTIF(AZ$3:AZ$28, "SYS")+COUNTIF(AZ$3:AZ$28, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="BA2" s="6">
@@ -1340,7 +1340,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 3:3))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 3:3))</f>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 3:3)+_xlfn.XLOOKUP("Extra size", $1:$1, 3:3)</f>
         <v>331</v>
       </c>
       <c r="G3" s="10" t="b">
@@ -1491,11 +1491,11 @@
         <v>0</v>
       </c>
       <c r="BD3" s="9">
-        <f>COUNTIF($G3:$BC3, "SYS")+COUNTIF($G3:$BC3, TRUE)</f>
+        <f t="shared" ref="BD3:BD28" si="1">COUNTIF($G3:$BC3, "SYS")+COUNTIF($G3:$BC3, TRUE)</f>
         <v>10</v>
       </c>
       <c r="BE3" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 3:3))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 3:3))</f>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 3:3)/_xlfn.XLOOKUP("Feature count", $1:$1, 3:3)</f>
         <v>30.4</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 4:4))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 4:4))</f>
+        <f t="shared" ref="F4:F28" si="2">_xlfn.XLOOKUP("Main size", $1:$1, 4:4)+_xlfn.XLOOKUP("Extra size", $1:$1, 4:4)</f>
         <v>512</v>
       </c>
       <c r="G4" s="10" t="b">
@@ -1667,11 +1667,11 @@
         <v>0</v>
       </c>
       <c r="BD4" s="9">
-        <f>COUNTIF($G4:$BC4, "SYS")+COUNTIF($G4:$BC4, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="BE4" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 4:4))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 4:4))</f>
+        <f t="shared" ref="BE4:BE28" si="3">_xlfn.XLOOKUP("Main size", $1:$1, 4:4)/_xlfn.XLOOKUP("Feature count", $1:$1, 4:4)</f>
         <v>31.75</v>
       </c>
     </row>
@@ -1686,14 +1686,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E5" s="3">
         <v>42</v>
       </c>
       <c r="F5" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 5:5))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 5:5))</f>
-        <v>509</v>
+        <f t="shared" si="2"/>
+        <v>506</v>
       </c>
       <c r="G5" s="10" t="b">
         <v>1</v>
@@ -1843,12 +1843,12 @@
         <v>0</v>
       </c>
       <c r="BD5" s="9">
-        <f>COUNTIF($G5:$BC5, "SYS")+COUNTIF($G5:$BC5, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="BE5" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 5:5))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 5:5))</f>
-        <v>33.357142857142854</v>
+        <f t="shared" si="3"/>
+        <v>33.142857142857146</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="34" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 6:6))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 6:6))</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="G6" s="10" t="b">
@@ -2019,11 +2019,11 @@
         <v>0</v>
       </c>
       <c r="BD6" s="9">
-        <f>COUNTIF($G6:$BC6, "SYS")+COUNTIF($G6:$BC6, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="BE6" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 6:6))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 6:6))</f>
+        <f t="shared" si="3"/>
         <v>34.25</v>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 7:7))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 7:7))</f>
+        <f t="shared" si="2"/>
         <v>471</v>
       </c>
       <c r="G7" s="10" t="b">
@@ -2195,11 +2195,11 @@
         <v>0</v>
       </c>
       <c r="BD7" s="9">
-        <f>COUNTIF($G7:$BC7, "SYS")+COUNTIF($G7:$BC7, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="BE7" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 7:7))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 7:7))</f>
+        <f t="shared" si="3"/>
         <v>36.230769230769234</v>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 8:8))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 8:8))</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="G8" s="10" t="b">
@@ -2371,11 +2371,11 @@
         <v>0</v>
       </c>
       <c r="BD8" s="9">
-        <f>COUNTIF($G8:$BC8, "SYS")+COUNTIF($G8:$BC8, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="BE8" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 8:8))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 8:8))</f>
+        <f t="shared" si="3"/>
         <v>41.833333333333336</v>
       </c>
     </row>
@@ -2396,7 +2396,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 9:9))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 9:9))</f>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
       <c r="G9" s="10" t="b">
@@ -2547,11 +2547,11 @@
         <v>0</v>
       </c>
       <c r="BD9" s="9">
-        <f>COUNTIF($G9:$BC9, "SYS")+COUNTIF($G9:$BC9, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="BE9" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 9:9))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 9:9))</f>
+        <f t="shared" si="3"/>
         <v>49.555555555555557</v>
       </c>
     </row>
@@ -2572,7 +2572,7 @@
         <v>91</v>
       </c>
       <c r="F10" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 10:10))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 10:10))</f>
+        <f t="shared" si="2"/>
         <v>1550</v>
       </c>
       <c r="G10" s="10" t="b">
@@ -2723,11 +2723,11 @@
         <v>0</v>
       </c>
       <c r="BD10" s="9">
-        <f>COUNTIF($G10:$BC10, "SYS")+COUNTIF($G10:$BC10, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="BE10" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 10:10))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 10:10))</f>
+        <f t="shared" si="3"/>
         <v>50.310344827586206</v>
       </c>
     </row>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 11:11))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 11:11))</f>
+        <f t="shared" si="2"/>
         <v>510</v>
       </c>
       <c r="G11" s="10" t="b">
@@ -2899,11 +2899,11 @@
         <v>0</v>
       </c>
       <c r="BD11" s="9">
-        <f>COUNTIF($G11:$BC11, "SYS")+COUNTIF($G11:$BC11, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BE11" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 11:11))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 11:11))</f>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
     </row>
@@ -2924,7 +2924,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 12:12))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 12:12))</f>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
       <c r="G12" s="10" t="b">
@@ -3075,11 +3075,11 @@
         <v>0</v>
       </c>
       <c r="BD12" s="9">
-        <f>COUNTIF($G12:$BC12, "SYS")+COUNTIF($G12:$BC12, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="BE12" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 12:12))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 12:12))</f>
+        <f t="shared" si="3"/>
         <v>54.555555555555557</v>
       </c>
     </row>
@@ -3100,7 +3100,7 @@
         <v>25</v>
       </c>
       <c r="F13" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 13:13))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 13:13))</f>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="G13" s="10" t="b">
@@ -3251,11 +3251,11 @@
         <v>0</v>
       </c>
       <c r="BD13" s="9">
-        <f>COUNTIF($G13:$BC13, "SYS")+COUNTIF($G13:$BC13, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="BE13" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 13:13))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 13:13))</f>
+        <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
     </row>
@@ -3276,7 +3276,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 14:14))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 14:14))</f>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
       <c r="G14" s="10" t="b">
@@ -3427,11 +3427,11 @@
         <v>0</v>
       </c>
       <c r="BD14" s="9">
-        <f>COUNTIF($G14:$BC14, "SYS")+COUNTIF($G14:$BC14, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="BE14" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 14:14))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 14:14))</f>
+        <f t="shared" si="3"/>
         <v>63.714285714285715</v>
       </c>
     </row>
@@ -3452,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 15:15))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 15:15))</f>
+        <f t="shared" si="2"/>
         <v>457</v>
       </c>
       <c r="G15" s="10" t="b">
@@ -3603,11 +3603,11 @@
         <v>0</v>
       </c>
       <c r="BD15" s="9">
-        <f>COUNTIF($G15:$BC15, "SYS")+COUNTIF($G15:$BC15, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="BE15" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 15:15))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 15:15))</f>
+        <f t="shared" si="3"/>
         <v>65.285714285714292</v>
       </c>
     </row>
@@ -3628,7 +3628,7 @@
         <v>234</v>
       </c>
       <c r="F16" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 16:16))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 16:16))</f>
+        <f t="shared" si="2"/>
         <v>1506</v>
       </c>
       <c r="G16" s="10" t="b">
@@ -3779,11 +3779,11 @@
         <v>0</v>
       </c>
       <c r="BD16" s="9">
-        <f>COUNTIF($G16:$BC16, "SYS")+COUNTIF($G16:$BC16, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="BE16" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 16:16))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 16:16))</f>
+        <f t="shared" si="3"/>
         <v>70.666666666666671</v>
       </c>
     </row>
@@ -3804,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 17:17))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 17:17))</f>
+        <f t="shared" si="2"/>
         <v>1358</v>
       </c>
       <c r="G17" s="10" t="b">
@@ -3955,11 +3955,11 @@
         <v>0</v>
       </c>
       <c r="BD17" s="9">
-        <f>COUNTIF($G17:$BC17, "SYS")+COUNTIF($G17:$BC17, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="BE17" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 17:17))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 17:17))</f>
+        <f t="shared" si="3"/>
         <v>84.875</v>
       </c>
     </row>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 18:18))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 18:18))</f>
+        <f t="shared" si="2"/>
         <v>2048</v>
       </c>
       <c r="G18" s="10" t="b">
@@ -4131,11 +4131,11 @@
         <v>0</v>
       </c>
       <c r="BD18" s="9">
-        <f>COUNTIF($G18:$BC18, "SYS")+COUNTIF($G18:$BC18, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="BE18" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 18:18))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 18:18))</f>
+        <f t="shared" si="3"/>
         <v>97.523809523809518</v>
       </c>
     </row>
@@ -4156,7 +4156,7 @@
         <v>123</v>
       </c>
       <c r="F19" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 19:19))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 19:19))</f>
+        <f t="shared" si="2"/>
         <v>1931</v>
       </c>
       <c r="G19" s="10" t="b">
@@ -4307,11 +4307,11 @@
         <v>0</v>
       </c>
       <c r="BD19" s="9">
-        <f>COUNTIF($G19:$BC19, "SYS")+COUNTIF($G19:$BC19, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="BE19" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 19:19))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 19:19))</f>
+        <f t="shared" si="3"/>
         <v>129.14285714285714</v>
       </c>
     </row>
@@ -4332,7 +4332,7 @@
         <v>1024</v>
       </c>
       <c r="F20" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 20:20))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 20:20))</f>
+        <f t="shared" si="2"/>
         <v>5040</v>
       </c>
       <c r="G20" s="10" t="b">
@@ -4483,11 +4483,11 @@
         <v>0</v>
       </c>
       <c r="BD20" s="9">
-        <f>COUNTIF($G20:$BC20, "SYS")+COUNTIF($G20:$BC20, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="BE20" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 20:20))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 20:20))</f>
+        <f t="shared" si="3"/>
         <v>133.86666666666667</v>
       </c>
     </row>
@@ -4508,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 21:21))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 21:21))</f>
+        <f t="shared" si="2"/>
         <v>1896</v>
       </c>
       <c r="G21" s="10" t="b">
@@ -4659,11 +4659,11 @@
         <v>0</v>
       </c>
       <c r="BD21" s="9">
-        <f>COUNTIF($G21:$BC21, "SYS")+COUNTIF($G21:$BC21, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="BE21" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 21:21))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 21:21))</f>
+        <f t="shared" si="3"/>
         <v>135.42857142857142</v>
       </c>
     </row>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 22:22))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 22:22))</f>
+        <f t="shared" si="2"/>
         <v>2738</v>
       </c>
       <c r="G22" s="10" t="b">
@@ -4835,11 +4835,11 @@
         <v>0</v>
       </c>
       <c r="BD22" s="9">
-        <f>COUNTIF($G22:$BC22, "SYS")+COUNTIF($G22:$BC22, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="BE22" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 22:22))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 22:22))</f>
+        <f t="shared" si="3"/>
         <v>152.11111111111111</v>
       </c>
     </row>
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 23:23))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 23:23))</f>
+        <f t="shared" si="2"/>
         <v>3998</v>
       </c>
       <c r="G23" s="10" t="b">
@@ -5011,11 +5011,11 @@
         <v>0</v>
       </c>
       <c r="BD23" s="9">
-        <f>COUNTIF($G23:$BC23, "SYS")+COUNTIF($G23:$BC23, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="BE23" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 23:23))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 23:23))</f>
+        <f t="shared" si="3"/>
         <v>159.91999999999999</v>
       </c>
     </row>
@@ -5036,7 +5036,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 24:24))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 24:24))</f>
+        <f t="shared" si="2"/>
         <v>2824</v>
       </c>
       <c r="G24" s="10" t="b">
@@ -5187,11 +5187,11 @@
         <v>0</v>
       </c>
       <c r="BD24" s="9">
-        <f>COUNTIF($G24:$BC24, "SYS")+COUNTIF($G24:$BC24, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="BE24" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 24:24))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 24:24))</f>
+        <f t="shared" si="3"/>
         <v>166.11764705882354</v>
       </c>
     </row>
@@ -5212,7 +5212,7 @@
         <v>100</v>
       </c>
       <c r="F25" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 25:25))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 25:25))</f>
+        <f t="shared" si="2"/>
         <v>2810</v>
       </c>
       <c r="G25" s="10" t="b">
@@ -5363,11 +5363,11 @@
         <v>0</v>
       </c>
       <c r="BD25" s="9">
-        <f>COUNTIF($G25:$BC25, "SYS")+COUNTIF($G25:$BC25, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="BE25" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 25:25))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 25:25))</f>
+        <f t="shared" si="3"/>
         <v>169.375</v>
       </c>
     </row>
@@ -5388,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 26:26))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 26:26))</f>
+        <f t="shared" si="2"/>
         <v>4095</v>
       </c>
       <c r="G26" s="10" t="b">
@@ -5539,11 +5539,11 @@
         <v>0</v>
       </c>
       <c r="BD26" s="9">
-        <f>COUNTIF($G26:$BC26, "SYS")+COUNTIF($G26:$BC26, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="BE26" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 26:26))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 26:26))</f>
+        <f t="shared" si="3"/>
         <v>178.04347826086956</v>
       </c>
     </row>
@@ -5564,7 +5564,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 27:27))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 27:27))</f>
+        <f t="shared" si="2"/>
         <v>2882</v>
       </c>
       <c r="G27" s="10" t="b">
@@ -5715,11 +5715,11 @@
         <v>0</v>
       </c>
       <c r="BD27" s="9">
-        <f>COUNTIF($G27:$BC27, "SYS")+COUNTIF($G27:$BC27, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="BE27" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 27:27))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 27:27))</f>
+        <f t="shared" si="3"/>
         <v>180.125</v>
       </c>
     </row>
@@ -5740,7 +5740,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="3">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 28:28))+_xlfn.SINGLE(_xlfn.XLOOKUP("Extra Size", $1:$1, 28:28))</f>
+        <f t="shared" si="2"/>
         <v>4002</v>
       </c>
       <c r="G28" s="10" t="b">
@@ -5891,11 +5891,11 @@
         <v>1</v>
       </c>
       <c r="BD28" s="9">
-        <f>COUNTIF($G28:$BC28, "SYS")+COUNTIF($G28:$BC28, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="BE28" s="4">
-        <f>_xlfn.SINGLE(_xlfn.XLOOKUP("Main Size", $1:$1, 28:28))/_xlfn.SINGLE(_xlfn.XLOOKUP("Feature Count", $1:$1, 28:28))</f>
+        <f t="shared" si="3"/>
         <v>190.57142857142858</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Archived 5 more programs
</commit_message>
<xml_diff>
--- a/tetris-4k-archive.xlsx
+++ b/tetris-4k-archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493d989091475df7/Personal/GitHub/tetris4karchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="314" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A62669B1-C19F-9847-86C3-43CD01DF2B45}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B0F1385-463D-CB48-AA2F-AC09E5997C7E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21140" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>notjagan</t>
   </si>
   <si>
-    <t>https://codegolf.stackexchange.com/a/121396/120787</t>
-  </si>
-  <si>
     <t>https://codegolf.stackexchange.com/a/11650/120787</t>
   </si>
   <si>
@@ -161,21 +158,12 @@
     <t>shikhin</t>
   </si>
   <si>
-    <t>https://github.com/shikhin/tetranglix</t>
-  </si>
-  <si>
     <t>https://codegolf.stackexchange.com/a/167445/120787</t>
   </si>
   <si>
     <t>Andrew March</t>
   </si>
   <si>
-    <t>http://www.p01.org/256b_tetris_theme</t>
-  </si>
-  <si>
-    <t>https://joriszwart.nl/games/javascript-tetris-1.5kb</t>
-  </si>
-  <si>
     <t>https://github.com/michowski/tetris-light</t>
   </si>
   <si>
@@ -203,9 +191,6 @@
     <t>wiesi</t>
   </si>
   <si>
-    <t>https://github.com/netspooky/hardcode/tree/master/02048/dos/1.32kb%20tetris</t>
-  </si>
-  <si>
     <t>Vzub Pnukem</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t>https://playdosgames.com/online/smalltetris</t>
   </si>
   <si>
-    <t>https://nineteendo.github.io/tetris4karchive/tinytetris</t>
-  </si>
-  <si>
     <t>Daniel Etzold</t>
   </si>
   <si>
@@ -390,6 +372,24 @@
   </si>
   <si>
     <t>https://nineteendo.github.io/tetris4karchive/tetranglix</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tiny-tetris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/256b-tetris-theme</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetranglix-2</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/binary-tetris-3</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/1.5kb-tetris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/1.32kb-tetris</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
   <dimension ref="A1:BF28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,46 +948,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>11</v>
@@ -996,34 +996,34 @@
         <v>9</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="AB1" s="5" t="s">
         <v>8</v>
@@ -1035,85 +1035,85 @@
         <v>24</v>
       </c>
       <c r="AE1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="AO1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="AP1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU1" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="AV1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="AW1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="AZ1" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE1" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="BF1" s="2"/>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="S2" s="6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T2" s="6">
         <f t="shared" si="0"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="W2" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X2" s="6">
         <f t="shared" si="0"/>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="3" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>26</v>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="BD3" s="9">
-        <f t="shared" ref="BD3:BD28" si="1">COUNTIF($G3:$BC3, "SYS")+COUNTIF($G3:$BC3, TRUE)</f>
+        <f>COUNTIF($G3:$BC3, "SYS")+COUNTIF($G3:$BC3, TRUE)</f>
         <v>10</v>
       </c>
       <c r="BE3" s="4">
@@ -1501,7 +1501,7 @@
     </row>
     <row r="4" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>15</v>
@@ -1516,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F28" si="2">_xlfn.XLOOKUP("Main size", $1:$1, 4:4)+_xlfn.XLOOKUP("Extra size", $1:$1, 4:4)</f>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 4:4)+_xlfn.XLOOKUP("Extra size", $1:$1, 4:4)</f>
         <v>512</v>
       </c>
       <c r="G4" s="10" t="b">
@@ -1667,17 +1667,17 @@
         <v>0</v>
       </c>
       <c r="BD4" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G4:$BC4, "SYS")+COUNTIF($G4:$BC4, TRUE)</f>
         <v>16</v>
       </c>
       <c r="BE4" s="4">
-        <f t="shared" ref="BE4:BE28" si="3">_xlfn.XLOOKUP("Main size", $1:$1, 4:4)/_xlfn.XLOOKUP("Feature count", $1:$1, 4:4)</f>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 4:4)/_xlfn.XLOOKUP("Feature count", $1:$1, 4:4)</f>
         <v>31.75</v>
       </c>
     </row>
     <row r="5" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
@@ -1692,7 +1692,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 5:5)+_xlfn.XLOOKUP("Extra size", $1:$1, 5:5)</f>
         <v>506</v>
       </c>
       <c r="G5" s="10" t="b">
@@ -1843,17 +1843,17 @@
         <v>0</v>
       </c>
       <c r="BD5" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G5:$BC5, "SYS")+COUNTIF($G5:$BC5, TRUE)</f>
         <v>14</v>
       </c>
       <c r="BE5" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 5:5)/_xlfn.XLOOKUP("Feature count", $1:$1, 5:5)</f>
         <v>33.142857142857146</v>
       </c>
     </row>
     <row r="6" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
@@ -1868,7 +1868,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 6:6)+_xlfn.XLOOKUP("Extra size", $1:$1, 6:6)</f>
         <v>300</v>
       </c>
       <c r="G6" s="10" t="b">
@@ -2019,20 +2019,20 @@
         <v>0</v>
       </c>
       <c r="BD6" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G6:$BC6, "SYS")+COUNTIF($G6:$BC6, TRUE)</f>
         <v>8</v>
       </c>
       <c r="BE6" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 6:6)/_xlfn.XLOOKUP("Feature count", $1:$1, 6:6)</f>
         <v>34.25</v>
       </c>
     </row>
     <row r="7" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>6</v>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 7:7)+_xlfn.XLOOKUP("Extra size", $1:$1, 7:7)</f>
         <v>471</v>
       </c>
       <c r="G7" s="10" t="b">
@@ -2195,17 +2195,17 @@
         <v>0</v>
       </c>
       <c r="BD7" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G7:$BC7, "SYS")+COUNTIF($G7:$BC7, TRUE)</f>
         <v>13</v>
       </c>
       <c r="BE7" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 7:7)/_xlfn.XLOOKUP("Feature count", $1:$1, 7:7)</f>
         <v>36.230769230769234</v>
       </c>
     </row>
     <row r="8" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>14</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 8:8)+_xlfn.XLOOKUP("Extra size", $1:$1, 8:8)</f>
         <v>251</v>
       </c>
       <c r="G8" s="10" t="b">
@@ -2371,20 +2371,20 @@
         <v>0</v>
       </c>
       <c r="BD8" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G8:$BC8, "SYS")+COUNTIF($G8:$BC8, TRUE)</f>
         <v>6</v>
       </c>
       <c r="BE8" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 8:8)/_xlfn.XLOOKUP("Feature count", $1:$1, 8:8)</f>
         <v>41.833333333333336</v>
       </c>
     </row>
     <row r="9" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>6</v>
@@ -2396,7 +2396,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 9:9)+_xlfn.XLOOKUP("Extra size", $1:$1, 9:9)</f>
         <v>512</v>
       </c>
       <c r="G9" s="10" t="b">
@@ -2547,17 +2547,17 @@
         <v>0</v>
       </c>
       <c r="BD9" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G9:$BC9, "SYS")+COUNTIF($G9:$BC9, TRUE)</f>
         <v>9</v>
       </c>
       <c r="BE9" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 9:9)/_xlfn.XLOOKUP("Feature count", $1:$1, 9:9)</f>
         <v>49.555555555555557</v>
       </c>
     </row>
     <row r="10" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>2</v>
@@ -2572,7 +2572,7 @@
         <v>91</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 10:10)+_xlfn.XLOOKUP("Extra size", $1:$1, 10:10)</f>
         <v>1550</v>
       </c>
       <c r="G10" s="10" t="b">
@@ -2723,20 +2723,20 @@
         <v>0</v>
       </c>
       <c r="BD10" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G10:$BC10, "SYS")+COUNTIF($G10:$BC10, TRUE)</f>
         <v>29</v>
       </c>
       <c r="BE10" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 10:10)/_xlfn.XLOOKUP("Feature count", $1:$1, 10:10)</f>
         <v>50.310344827586206</v>
       </c>
     </row>
     <row r="11" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>6</v>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 11:11)+_xlfn.XLOOKUP("Extra size", $1:$1, 11:11)</f>
         <v>510</v>
       </c>
       <c r="G11" s="10" t="b">
@@ -2899,20 +2899,20 @@
         <v>0</v>
       </c>
       <c r="BD11" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G11:$BC11, "SYS")+COUNTIF($G11:$BC11, TRUE)</f>
         <v>10</v>
       </c>
       <c r="BE11" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 11:11)/_xlfn.XLOOKUP("Feature count", $1:$1, 11:11)</f>
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
@@ -2924,7 +2924,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 12:12)+_xlfn.XLOOKUP("Extra size", $1:$1, 12:12)</f>
         <v>512</v>
       </c>
       <c r="G12" s="10" t="b">
@@ -3075,17 +3075,17 @@
         <v>0</v>
       </c>
       <c r="BD12" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G12:$BC12, "SYS")+COUNTIF($G12:$BC12, TRUE)</f>
         <v>9</v>
       </c>
       <c r="BE12" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 12:12)/_xlfn.XLOOKUP("Feature count", $1:$1, 12:12)</f>
         <v>54.555555555555557</v>
       </c>
     </row>
     <row r="13" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>21</v>
@@ -3094,14 +3094,14 @@
         <v>4</v>
       </c>
       <c r="D13" s="3">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E13" s="3">
         <v>25</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="2"/>
-        <v>255</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)+_xlfn.XLOOKUP("Extra size", $1:$1, 13:13)</f>
+        <v>252</v>
       </c>
       <c r="G13" s="10" t="b">
         <v>0</v>
@@ -3251,20 +3251,20 @@
         <v>0</v>
       </c>
       <c r="BD13" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G13:$BC13, "SYS")+COUNTIF($G13:$BC13, TRUE)</f>
         <v>4</v>
       </c>
       <c r="BE13" s="4">
-        <f t="shared" si="3"/>
-        <v>57.5</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)/_xlfn.XLOOKUP("Feature count", $1:$1, 13:13)</f>
+        <v>56.75</v>
       </c>
     </row>
-    <row r="14" spans="1:58" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>6</v>
@@ -3276,7 +3276,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 14:14)+_xlfn.XLOOKUP("Extra size", $1:$1, 14:14)</f>
         <v>512</v>
       </c>
       <c r="G14" s="10" t="b">
@@ -3427,17 +3427,17 @@
         <v>0</v>
       </c>
       <c r="BD14" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G14:$BC14, "SYS")+COUNTIF($G14:$BC14, TRUE)</f>
         <v>7</v>
       </c>
       <c r="BE14" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 14:14)/_xlfn.XLOOKUP("Feature count", $1:$1, 14:14)</f>
         <v>63.714285714285715</v>
       </c>
     </row>
     <row r="15" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>30</v>
@@ -3452,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 15:15)+_xlfn.XLOOKUP("Extra size", $1:$1, 15:15)</f>
         <v>457</v>
       </c>
       <c r="G15" s="10" t="b">
@@ -3603,17 +3603,17 @@
         <v>0</v>
       </c>
       <c r="BD15" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G15:$BC15, "SYS")+COUNTIF($G15:$BC15, TRUE)</f>
         <v>7</v>
       </c>
       <c r="BE15" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 15:15)/_xlfn.XLOOKUP("Feature count", $1:$1, 15:15)</f>
         <v>65.285714285714292</v>
       </c>
     </row>
     <row r="16" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>12</v>
@@ -3622,14 +3622,14 @@
         <v>4</v>
       </c>
       <c r="D16" s="3">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="E16" s="3">
         <v>234</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="2"/>
-        <v>1506</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 16:16)+_xlfn.XLOOKUP("Extra size", $1:$1, 16:16)</f>
+        <v>1503</v>
       </c>
       <c r="G16" s="10" t="b">
         <v>1</v>
@@ -3668,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="10" t="b">
         <v>1</v>
@@ -3680,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="W16" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="10" t="b">
         <v>0</v>
@@ -3779,20 +3779,20 @@
         <v>0</v>
       </c>
       <c r="BD16" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G16:$BC16, "SYS")+COUNTIF($G16:$BC16, TRUE)</f>
         <v>18</v>
       </c>
       <c r="BE16" s="4">
-        <f t="shared" si="3"/>
-        <v>70.666666666666671</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 16:16)/_xlfn.XLOOKUP("Feature count", $1:$1, 16:16)</f>
+        <v>70.5</v>
       </c>
     </row>
     <row r="17" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>6</v>
@@ -3804,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 17:17)+_xlfn.XLOOKUP("Extra size", $1:$1, 17:17)</f>
         <v>1358</v>
       </c>
       <c r="G17" s="10" t="b">
@@ -3955,20 +3955,20 @@
         <v>0</v>
       </c>
       <c r="BD17" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G17:$BC17, "SYS")+COUNTIF($G17:$BC17, TRUE)</f>
         <v>16</v>
       </c>
       <c r="BE17" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 17:17)/_xlfn.XLOOKUP("Feature count", $1:$1, 17:17)</f>
         <v>84.875</v>
       </c>
     </row>
     <row r="18" spans="1:57" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>6</v>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 18:18)+_xlfn.XLOOKUP("Extra size", $1:$1, 18:18)</f>
         <v>2048</v>
       </c>
       <c r="G18" s="10" t="b">
@@ -4131,17 +4131,17 @@
         <v>0</v>
       </c>
       <c r="BD18" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G18:$BC18, "SYS")+COUNTIF($G18:$BC18, TRUE)</f>
         <v>21</v>
       </c>
       <c r="BE18" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 18:18)/_xlfn.XLOOKUP("Feature count", $1:$1, 18:18)</f>
         <v>97.523809523809518</v>
       </c>
     </row>
     <row r="19" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>17</v>
@@ -4150,14 +4150,14 @@
         <v>4</v>
       </c>
       <c r="D19" s="3">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="E19" s="3">
         <v>123</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="2"/>
-        <v>1931</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 19:19)+_xlfn.XLOOKUP("Extra size", $1:$1, 19:19)</f>
+        <v>1928</v>
       </c>
       <c r="G19" s="10" t="b">
         <v>1</v>
@@ -4307,20 +4307,20 @@
         <v>0</v>
       </c>
       <c r="BD19" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G19:$BC19, "SYS")+COUNTIF($G19:$BC19, TRUE)</f>
         <v>14</v>
       </c>
       <c r="BE19" s="4">
-        <f t="shared" si="3"/>
-        <v>129.14285714285714</v>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 19:19)/_xlfn.XLOOKUP("Feature count", $1:$1, 19:19)</f>
+        <v>128.92857142857142</v>
       </c>
     </row>
     <row r="20" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>4</v>
@@ -4332,7 +4332,7 @@
         <v>1024</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 20:20)+_xlfn.XLOOKUP("Extra size", $1:$1, 20:20)</f>
         <v>5040</v>
       </c>
       <c r="G20" s="10" t="b">
@@ -4483,11 +4483,11 @@
         <v>0</v>
       </c>
       <c r="BD20" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G20:$BC20, "SYS")+COUNTIF($G20:$BC20, TRUE)</f>
         <v>30</v>
       </c>
       <c r="BE20" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 20:20)/_xlfn.XLOOKUP("Feature count", $1:$1, 20:20)</f>
         <v>133.86666666666667</v>
       </c>
     </row>
@@ -4508,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 21:21)+_xlfn.XLOOKUP("Extra size", $1:$1, 21:21)</f>
         <v>1896</v>
       </c>
       <c r="G21" s="10" t="b">
@@ -4659,11 +4659,11 @@
         <v>0</v>
       </c>
       <c r="BD21" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G21:$BC21, "SYS")+COUNTIF($G21:$BC21, TRUE)</f>
         <v>14</v>
       </c>
       <c r="BE21" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 21:21)/_xlfn.XLOOKUP("Feature count", $1:$1, 21:21)</f>
         <v>135.42857142857142</v>
       </c>
     </row>
@@ -4672,7 +4672,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>27</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)+_xlfn.XLOOKUP("Extra size", $1:$1, 22:22)</f>
         <v>2738</v>
       </c>
       <c r="G22" s="10" t="b">
@@ -4835,23 +4835,23 @@
         <v>0</v>
       </c>
       <c r="BD22" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G22:$BC22, "SYS")+COUNTIF($G22:$BC22, TRUE)</f>
         <v>18</v>
       </c>
       <c r="BE22" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)/_xlfn.XLOOKUP("Feature count", $1:$1, 22:22)</f>
         <v>152.11111111111111</v>
       </c>
     </row>
     <row r="23" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3">
         <v>3998</v>
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 23:23)+_xlfn.XLOOKUP("Extra size", $1:$1, 23:23)</f>
         <v>3998</v>
       </c>
       <c r="G23" s="10" t="b">
@@ -5011,11 +5011,11 @@
         <v>0</v>
       </c>
       <c r="BD23" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G23:$BC23, "SYS")+COUNTIF($G23:$BC23, TRUE)</f>
         <v>25</v>
       </c>
       <c r="BE23" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 23:23)/_xlfn.XLOOKUP("Feature count", $1:$1, 23:23)</f>
         <v>159.91999999999999</v>
       </c>
     </row>
@@ -5024,7 +5024,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>5</v>
@@ -5036,7 +5036,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 24:24)+_xlfn.XLOOKUP("Extra size", $1:$1, 24:24)</f>
         <v>2824</v>
       </c>
       <c r="G24" s="10" t="b">
@@ -5187,20 +5187,20 @@
         <v>0</v>
       </c>
       <c r="BD24" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G24:$BC24, "SYS")+COUNTIF($G24:$BC24, TRUE)</f>
         <v>17</v>
       </c>
       <c r="BE24" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 24:24)/_xlfn.XLOOKUP("Feature count", $1:$1, 24:24)</f>
         <v>166.11764705882354</v>
       </c>
     </row>
     <row r="25" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>4</v>
@@ -5212,7 +5212,7 @@
         <v>100</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 25:25)+_xlfn.XLOOKUP("Extra size", $1:$1, 25:25)</f>
         <v>2810</v>
       </c>
       <c r="G25" s="10" t="b">
@@ -5363,23 +5363,23 @@
         <v>0</v>
       </c>
       <c r="BD25" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G25:$BC25, "SYS")+COUNTIF($G25:$BC25, TRUE)</f>
         <v>16</v>
       </c>
       <c r="BE25" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 25:25)/_xlfn.XLOOKUP("Feature count", $1:$1, 25:25)</f>
         <v>169.375</v>
       </c>
     </row>
     <row r="26" spans="1:57" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3">
         <v>4095</v>
@@ -5388,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)+_xlfn.XLOOKUP("Extra size", $1:$1, 26:26)</f>
         <v>4095</v>
       </c>
       <c r="G26" s="10" t="b">
@@ -5539,23 +5539,23 @@
         <v>0</v>
       </c>
       <c r="BD26" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G26:$BC26, "SYS")+COUNTIF($G26:$BC26, TRUE)</f>
         <v>23</v>
       </c>
       <c r="BE26" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)/_xlfn.XLOOKUP("Feature count", $1:$1, 26:26)</f>
         <v>178.04347826086956</v>
       </c>
     </row>
     <row r="27" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="D27" s="3">
         <v>2882</v>
@@ -5564,7 +5564,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)+_xlfn.XLOOKUP("Extra size", $1:$1, 27:27)</f>
         <v>2882</v>
       </c>
       <c r="G27" s="10" t="b">
@@ -5715,23 +5715,23 @@
         <v>0</v>
       </c>
       <c r="BD27" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G27:$BC27, "SYS")+COUNTIF($G27:$BC27, TRUE)</f>
         <v>16</v>
       </c>
       <c r="BE27" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)/_xlfn.XLOOKUP("Feature count", $1:$1, 27:27)</f>
         <v>180.125</v>
       </c>
     </row>
     <row r="28" spans="1:57" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3">
         <v>4002</v>
@@ -5740,7 +5740,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="2"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 28:28)+_xlfn.XLOOKUP("Extra size", $1:$1, 28:28)</f>
         <v>4002</v>
       </c>
       <c r="G28" s="10" t="b">
@@ -5891,11 +5891,11 @@
         <v>1</v>
       </c>
       <c r="BD28" s="9">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($G28:$BC28, "SYS")+COUNTIF($G28:$BC28, TRUE)</f>
         <v>21</v>
       </c>
       <c r="BE28" s="4">
-        <f t="shared" si="3"/>
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 28:28)/_xlfn.XLOOKUP("Feature count", $1:$1, 28:28)</f>
         <v>190.57142857142858</v>
       </c>
     </row>
@@ -5981,23 +5981,23 @@
     <hyperlink ref="A5" r:id="rId6" xr:uid="{D6CABB3D-301E-5A48-8390-5B6D8D98891E}"/>
     <hyperlink ref="A6" r:id="rId7" xr:uid="{1EAE54DC-A089-B24E-A04A-825543C48D1A}"/>
     <hyperlink ref="A13" r:id="rId8" xr:uid="{65802411-1B8E-064F-A6D7-DAD404DC6F66}"/>
-    <hyperlink ref="A16" r:id="rId9" xr:uid="{7FBBD806-6032-6042-9A3F-9BB930A440B9}"/>
-    <hyperlink ref="A19" r:id="rId10" xr:uid="{B15F6BAD-35BC-2A4D-A9F9-E3397D6C9F57}"/>
-    <hyperlink ref="A20" r:id="rId11" xr:uid="{A76D4E5E-9C61-C846-BF68-39EA20E19271}"/>
-    <hyperlink ref="A25" r:id="rId12" xr:uid="{271A3F43-6A28-9044-9B77-55CB67E8E604}"/>
-    <hyperlink ref="A27" r:id="rId13" xr:uid="{3319FE9B-1572-7B45-A51A-8631F49908F5}"/>
-    <hyperlink ref="A22" r:id="rId14" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
-    <hyperlink ref="A15" r:id="rId15" xr:uid="{F4CDBBC8-4471-9C45-8656-76234F7A7EE4}"/>
-    <hyperlink ref="A10" r:id="rId16" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
-    <hyperlink ref="A24" r:id="rId17" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
-    <hyperlink ref="A26" r:id="rId18" xr:uid="{BE81C522-7811-534B-B250-C27D6ED80E13}"/>
-    <hyperlink ref="A17" r:id="rId19" xr:uid="{080E4C73-46F1-F445-93A2-BDE904141286}"/>
-    <hyperlink ref="A11" r:id="rId20" xr:uid="{F2854865-7589-3148-9BD0-694117F0C02A}"/>
-    <hyperlink ref="A18" r:id="rId21" xr:uid="{7A0C5CE4-FDBB-C142-89E0-609051079143}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{B27A7A0A-1947-624B-A135-AC2E4FA9DCDF}"/>
-    <hyperlink ref="A7" r:id="rId23" xr:uid="{0C291FB0-BA8C-E141-98A4-91A6B6DD9884}"/>
-    <hyperlink ref="A9" r:id="rId24" xr:uid="{2F1BE129-94F7-DB45-B74A-D5DECFC8BD1F}"/>
-    <hyperlink ref="A12" r:id="rId25" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>
+    <hyperlink ref="A19" r:id="rId9" xr:uid="{B15F6BAD-35BC-2A4D-A9F9-E3397D6C9F57}"/>
+    <hyperlink ref="A20" r:id="rId10" xr:uid="{A76D4E5E-9C61-C846-BF68-39EA20E19271}"/>
+    <hyperlink ref="A25" r:id="rId11" xr:uid="{271A3F43-6A28-9044-9B77-55CB67E8E604}"/>
+    <hyperlink ref="A27" r:id="rId12" xr:uid="{3319FE9B-1572-7B45-A51A-8631F49908F5}"/>
+    <hyperlink ref="A22" r:id="rId13" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
+    <hyperlink ref="A10" r:id="rId14" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
+    <hyperlink ref="A24" r:id="rId15" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
+    <hyperlink ref="A26" r:id="rId16" xr:uid="{BE81C522-7811-534B-B250-C27D6ED80E13}"/>
+    <hyperlink ref="A11" r:id="rId17" xr:uid="{F2854865-7589-3148-9BD0-694117F0C02A}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{7A0C5CE4-FDBB-C142-89E0-609051079143}"/>
+    <hyperlink ref="A23" r:id="rId19" xr:uid="{B27A7A0A-1947-624B-A135-AC2E4FA9DCDF}"/>
+    <hyperlink ref="A7" r:id="rId20" xr:uid="{0C291FB0-BA8C-E141-98A4-91A6B6DD9884}"/>
+    <hyperlink ref="A9" r:id="rId21" xr:uid="{2F1BE129-94F7-DB45-B74A-D5DECFC8BD1F}"/>
+    <hyperlink ref="A12" r:id="rId22" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>
+    <hyperlink ref="A15" r:id="rId23" xr:uid="{BBFDB1C2-F4D5-9F4F-9AB4-84F69F8E341F}"/>
+    <hyperlink ref="A16" r:id="rId24" xr:uid="{47C1315B-4443-9B43-9DB9-33643DFA677C}"/>
+    <hyperlink ref="A17" r:id="rId25" xr:uid="{C77570FF-B176-1F4E-AC94-8C167340C676}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Archived 12 more programs
</commit_message>
<xml_diff>
--- a/tetris-4k-archive.xlsx
+++ b/tetris-4k-archive.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493d989091475df7/Personal/GitHub/tetris4karchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B0F1385-463D-CB48-AA2F-AC09E5997C7E}"/>
+  <xr:revisionPtr revIDLastSave="526" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33611244-5C0C-EC42-AD36-B52C09D9A1CA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21140" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$BE$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$BF$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>Url</t>
   </si>
   <si>
-    <t>https://ticalc.org/archives/files/fileinfo/371/37183.html</t>
-  </si>
-  <si>
     <t>Nice Zombies</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Arek Michowski</t>
   </si>
   <si>
-    <t>http://sebastianmihai.com/asmtris.html</t>
-  </si>
-  <si>
     <t>Sebastian Mihai</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>Mathieu Henri</t>
   </si>
   <si>
-    <t>SFX</t>
-  </si>
-  <si>
     <t>Retry</t>
   </si>
   <si>
@@ -125,18 +116,12 @@
     <t>Pascal</t>
   </si>
   <si>
-    <t>https://codegolf.stackexchange.com/a/11548/120787</t>
-  </si>
-  <si>
     <t>Python</t>
   </si>
   <si>
     <t>notjagan</t>
   </si>
   <si>
-    <t>https://codegolf.stackexchange.com/a/11650/120787</t>
-  </si>
-  <si>
     <t>mniip</t>
   </si>
   <si>
@@ -158,18 +143,9 @@
     <t>shikhin</t>
   </si>
   <si>
-    <t>https://codegolf.stackexchange.com/a/167445/120787</t>
-  </si>
-  <si>
     <t>Andrew March</t>
   </si>
   <si>
-    <t>https://github.com/michowski/tetris-light</t>
-  </si>
-  <si>
-    <t>https://github.com/ttencate/tis</t>
-  </si>
-  <si>
     <t>Petr Blahos</t>
   </si>
   <si>
@@ -179,15 +155,9 @@
     <t>Shadows</t>
   </si>
   <si>
-    <t>https://github.com/netspooky/hardcode/tree/master/04096/java/t4k</t>
-  </si>
-  <si>
     <t>flub</t>
   </si>
   <si>
-    <t>https://github.com/netspooky/hardcode/tree/master/04096/java/tetris</t>
-  </si>
-  <si>
     <t>wiesi</t>
   </si>
   <si>
@@ -239,9 +209,6 @@
     <t>Line clear points</t>
   </si>
   <si>
-    <t>Next queue</t>
-  </si>
-  <si>
     <t>Hard drop</t>
   </si>
   <si>
@@ -281,9 +248,6 @@
     <t>Easter eggs</t>
   </si>
   <si>
-    <t>Hold queue</t>
-  </si>
-  <si>
     <t>Height selection</t>
   </si>
   <si>
@@ -338,9 +302,6 @@
     <t>https://nineteendo.github.io/tetris4karchive/binary-tetris</t>
   </si>
   <si>
-    <t>https://nineteendo.github.io/tetris4karchive/tetros105</t>
-  </si>
-  <si>
     <t>https://nineteendo.github.io/tetris4karchive/mini-tetris</t>
   </si>
   <si>
@@ -350,12 +311,6 @@
     <t>https://nineteendo.github.io/tetris4karchive/tinytris</t>
   </si>
   <si>
-    <t>https://web.archive.org/web/20201007111205/https://sites.google.com/site/petrsstuff/projects/4ktris</t>
-  </si>
-  <si>
-    <t>https://playdosgames.com/online/smalltetris</t>
-  </si>
-  <si>
     <t>Daniel Etzold</t>
   </si>
   <si>
@@ -390,6 +345,51 @@
   </si>
   <si>
     <t>https://nineteendo.github.io/tetris4karchive/1.32kb-tetris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetros-v105</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/small-tetris</t>
+  </si>
+  <si>
+    <t>Hold piece</t>
+  </si>
+  <si>
+    <t>Piece preview</t>
+  </si>
+  <si>
+    <t>Piece preview selection</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-light</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tis</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/asmtris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/another-tetris-4k</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-2</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-3</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-4</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-5</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/4k-tris</t>
+  </si>
+  <si>
+    <t>https://nineteendo.github.io/tetris4karchive/tetris-4k</t>
   </si>
 </sst>
 </file>
@@ -919,205 +919,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
-  <dimension ref="A1:BF28"/>
+  <dimension ref="A1:BG28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B2:B16"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1640625" customWidth="1"/>
-    <col min="14" max="41" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="6.1640625" customWidth="1"/>
-    <col min="45" max="54" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.1640625" customWidth="1"/>
-    <col min="56" max="56" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="108" width="10.83203125" customWidth="1"/>
+    <col min="4" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="42" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="46" width="6.1640625" customWidth="1"/>
+    <col min="47" max="55" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.1640625" customWidth="1"/>
+    <col min="57" max="57" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="109" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="1" customFormat="1" ht="104" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" s="1" customFormat="1" ht="104" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="U1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AL1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AO1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AR1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AX1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AZ1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="BA1" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="BE1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1129,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:BC2" si="0">COUNTIF(H$3:H$28, "SYS")+COUNTIF(H$3:H$28, TRUE)</f>
+        <f t="shared" ref="H2:BD2" si="0">COUNTIF(H$3:H$28, "SYS")+COUNTIF(H$3:H$28, TRUE)</f>
         <v>25</v>
       </c>
       <c r="I2" s="6">
@@ -1146,7 +1147,7 @@
       </c>
       <c r="L2" s="6">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" s="6">
         <f t="shared" si="0"/>
@@ -1266,7 +1267,7 @@
       </c>
       <c r="AP2" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AQ2" s="6">
         <f t="shared" si="0"/>
@@ -1278,11 +1279,11 @@
       </c>
       <c r="AS2" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT2" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU2" s="6">
         <f t="shared" si="0"/>
@@ -1294,23 +1295,23 @@
       </c>
       <c r="AW2" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX2" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AY2" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ2" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BA2" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB2" s="6">
         <f t="shared" si="0"/>
@@ -1320,18 +1321,22 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BD2" s="6"/>
+      <c r="BD2" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="BE2" s="6"/>
+      <c r="BF2" s="6"/>
     </row>
-    <row r="3" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3">
         <v>304</v>
@@ -1356,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L3" s="10" t="b">
         <v>1</v>
@@ -1365,13 +1370,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O3" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q3" s="10" t="b">
         <v>0</v>
@@ -1490,24 +1495,27 @@
       <c r="BC3" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD3" s="9">
-        <f>COUNTIF($G3:$BC3, "SYS")+COUNTIF($G3:$BC3, TRUE)</f>
+      <c r="BD3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="9">
+        <f>COUNTIF($G3:$BD3, "SYS")+COUNTIF($G3:$BD3, TRUE)</f>
         <v>10</v>
       </c>
-      <c r="BE3" s="4">
+      <c r="BF3" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 3:3)/_xlfn.XLOOKUP("Feature count", $1:$1, 3:3)</f>
         <v>30.4</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
         <v>508</v>
@@ -1666,24 +1674,27 @@
       <c r="BC4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD4" s="9">
-        <f>COUNTIF($G4:$BC4, "SYS")+COUNTIF($G4:$BC4, TRUE)</f>
+      <c r="BD4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="9">
+        <f>COUNTIF($G4:$BD4, "SYS")+COUNTIF($G4:$BD4, TRUE)</f>
         <v>16</v>
       </c>
-      <c r="BE4" s="4">
+      <c r="BF4" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 4:4)/_xlfn.XLOOKUP("Feature count", $1:$1, 4:4)</f>
         <v>31.75</v>
       </c>
     </row>
-    <row r="5" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>464</v>
@@ -1708,22 +1719,22 @@
         <v>1</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L5" s="10" t="b">
         <v>1</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O5" s="10" t="b">
         <v>0</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="10" t="b">
         <v>1</v>
@@ -1842,24 +1853,27 @@
       <c r="BC5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD5" s="9">
-        <f>COUNTIF($G5:$BC5, "SYS")+COUNTIF($G5:$BC5, TRUE)</f>
+      <c r="BD5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="9">
+        <f>COUNTIF($G5:$BD5, "SYS")+COUNTIF($G5:$BD5, TRUE)</f>
         <v>14</v>
       </c>
-      <c r="BE5" s="4">
+      <c r="BF5" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 5:5)/_xlfn.XLOOKUP("Feature count", $1:$1, 5:5)</f>
         <v>33.142857142857146</v>
       </c>
     </row>
-    <row r="6" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>4</v>
       </c>
       <c r="D6" s="3">
         <v>274</v>
@@ -1884,22 +1898,22 @@
         <v>0</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L6" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O6" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="10" t="b">
         <v>0</v>
@@ -2018,24 +2032,27 @@
       <c r="BC6" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD6" s="9">
-        <f>COUNTIF($G6:$BC6, "SYS")+COUNTIF($G6:$BC6, TRUE)</f>
+      <c r="BD6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="9">
+        <f>COUNTIF($G6:$BD6, "SYS")+COUNTIF($G6:$BD6, TRUE)</f>
         <v>8</v>
       </c>
-      <c r="BE6" s="4">
+      <c r="BF6" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 6:6)/_xlfn.XLOOKUP("Feature count", $1:$1, 6:6)</f>
         <v>34.25</v>
       </c>
     </row>
-    <row r="7" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
         <v>471</v>
@@ -2194,24 +2211,27 @@
       <c r="BC7" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD7" s="9">
-        <f>COUNTIF($G7:$BC7, "SYS")+COUNTIF($G7:$BC7, TRUE)</f>
+      <c r="BD7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="9">
+        <f>COUNTIF($G7:$BD7, "SYS")+COUNTIF($G7:$BD7, TRUE)</f>
         <v>13</v>
       </c>
-      <c r="BE7" s="4">
+      <c r="BF7" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 7:7)/_xlfn.XLOOKUP("Feature count", $1:$1, 7:7)</f>
         <v>36.230769230769234</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
         <v>251</v>
@@ -2370,24 +2390,27 @@
       <c r="BC8" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD8" s="9">
-        <f>COUNTIF($G8:$BC8, "SYS")+COUNTIF($G8:$BC8, TRUE)</f>
+      <c r="BD8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="9">
+        <f>COUNTIF($G8:$BD8, "SYS")+COUNTIF($G8:$BD8, TRUE)</f>
         <v>6</v>
       </c>
-      <c r="BE8" s="4">
+      <c r="BF8" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 8:8)/_xlfn.XLOOKUP("Feature count", $1:$1, 8:8)</f>
         <v>41.833333333333336</v>
       </c>
     </row>
-    <row r="9" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
         <v>446</v>
@@ -2546,24 +2569,27 @@
       <c r="BC9" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD9" s="9">
-        <f>COUNTIF($G9:$BC9, "SYS")+COUNTIF($G9:$BC9, TRUE)</f>
+      <c r="BD9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="9">
+        <f>COUNTIF($G9:$BD9, "SYS")+COUNTIF($G9:$BD9, TRUE)</f>
         <v>9</v>
       </c>
-      <c r="BE9" s="4">
+      <c r="BF9" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 9:9)/_xlfn.XLOOKUP("Feature count", $1:$1, 9:9)</f>
         <v>49.555555555555557</v>
       </c>
     </row>
-    <row r="10" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3">
         <v>1459</v>
@@ -2722,24 +2748,27 @@
       <c r="BC10" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD10" s="9">
-        <f>COUNTIF($G10:$BC10, "SYS")+COUNTIF($G10:$BC10, TRUE)</f>
+      <c r="BD10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="9">
+        <f>COUNTIF($G10:$BD10, "SYS")+COUNTIF($G10:$BD10, TRUE)</f>
         <v>29</v>
       </c>
-      <c r="BE10" s="4">
+      <c r="BF10" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 10:10)/_xlfn.XLOOKUP("Feature count", $1:$1, 10:10)</f>
         <v>50.310344827586206</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <v>510</v>
@@ -2898,24 +2927,27 @@
       <c r="BC11" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD11" s="9">
-        <f>COUNTIF($G11:$BC11, "SYS")+COUNTIF($G11:$BC11, TRUE)</f>
+      <c r="BD11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="9">
+        <f>COUNTIF($G11:$BD11, "SYS")+COUNTIF($G11:$BD11, TRUE)</f>
         <v>10</v>
       </c>
-      <c r="BE11" s="4">
+      <c r="BF11" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 11:11)/_xlfn.XLOOKUP("Feature count", $1:$1, 11:11)</f>
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <v>491</v>
@@ -3074,24 +3106,27 @@
       <c r="BC12" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD12" s="9">
-        <f>COUNTIF($G12:$BC12, "SYS")+COUNTIF($G12:$BC12, TRUE)</f>
+      <c r="BD12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE12" s="9">
+        <f>COUNTIF($G12:$BD12, "SYS")+COUNTIF($G12:$BD12, TRUE)</f>
         <v>9</v>
       </c>
-      <c r="BE12" s="4">
+      <c r="BF12" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 12:12)/_xlfn.XLOOKUP("Feature count", $1:$1, 12:12)</f>
         <v>54.555555555555557</v>
       </c>
     </row>
-    <row r="13" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3">
         <v>227</v>
@@ -3116,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L13" s="10" t="b">
         <v>0</v>
@@ -3125,13 +3160,13 @@
         <v>0</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O13" s="10" t="b">
         <v>0</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="10" t="b">
         <v>0</v>
@@ -3250,24 +3285,27 @@
       <c r="BC13" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD13" s="9">
-        <f>COUNTIF($G13:$BC13, "SYS")+COUNTIF($G13:$BC13, TRUE)</f>
+      <c r="BD13" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="9">
+        <f>COUNTIF($G13:$BD13, "SYS")+COUNTIF($G13:$BD13, TRUE)</f>
         <v>4</v>
       </c>
-      <c r="BE13" s="4">
+      <c r="BF13" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)/_xlfn.XLOOKUP("Feature count", $1:$1, 13:13)</f>
         <v>56.75</v>
       </c>
     </row>
-    <row r="14" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <v>446</v>
@@ -3426,24 +3464,27 @@
       <c r="BC14" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD14" s="9">
-        <f>COUNTIF($G14:$BC14, "SYS")+COUNTIF($G14:$BC14, TRUE)</f>
+      <c r="BD14" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE14" s="9">
+        <f>COUNTIF($G14:$BD14, "SYS")+COUNTIF($G14:$BD14, TRUE)</f>
         <v>7</v>
       </c>
-      <c r="BE14" s="4">
+      <c r="BF14" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 14:14)/_xlfn.XLOOKUP("Feature count", $1:$1, 14:14)</f>
         <v>63.714285714285715</v>
       </c>
     </row>
-    <row r="15" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3">
         <v>457</v>
@@ -3477,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O15" s="10" t="b">
         <v>1</v>
@@ -3602,24 +3643,27 @@
       <c r="BC15" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD15" s="9">
-        <f>COUNTIF($G15:$BC15, "SYS")+COUNTIF($G15:$BC15, TRUE)</f>
+      <c r="BD15" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE15" s="9">
+        <f>COUNTIF($G15:$BD15, "SYS")+COUNTIF($G15:$BD15, TRUE)</f>
         <v>7</v>
       </c>
-      <c r="BE15" s="4">
+      <c r="BF15" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 15:15)/_xlfn.XLOOKUP("Feature count", $1:$1, 15:15)</f>
         <v>65.285714285714292</v>
       </c>
     </row>
-    <row r="16" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3">
         <v>1269</v>
@@ -3644,22 +3688,22 @@
         <v>1</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L16" s="10" t="b">
         <v>1</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O16" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q16" s="10" t="b">
         <v>1</v>
@@ -3778,24 +3822,27 @@
       <c r="BC16" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD16" s="9">
-        <f>COUNTIF($G16:$BC16, "SYS")+COUNTIF($G16:$BC16, TRUE)</f>
+      <c r="BD16" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE16" s="9">
+        <f>COUNTIF($G16:$BD16, "SYS")+COUNTIF($G16:$BD16, TRUE)</f>
         <v>18</v>
       </c>
-      <c r="BE16" s="4">
+      <c r="BF16" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 16:16)/_xlfn.XLOOKUP("Feature count", $1:$1, 16:16)</f>
         <v>70.5</v>
       </c>
     </row>
-    <row r="17" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
         <v>1358</v>
@@ -3916,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="AQ17" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR17" s="10" t="b">
         <v>0</v>
@@ -3954,24 +4001,27 @@
       <c r="BC17" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD17" s="9">
-        <f>COUNTIF($G17:$BC17, "SYS")+COUNTIF($G17:$BC17, TRUE)</f>
-        <v>16</v>
-      </c>
-      <c r="BE17" s="4">
+      <c r="BD17" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="9">
+        <f>COUNTIF($G17:$BD17, "SYS")+COUNTIF($G17:$BD17, TRUE)</f>
+        <v>17</v>
+      </c>
+      <c r="BF17" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 17:17)/_xlfn.XLOOKUP("Feature count", $1:$1, 17:17)</f>
-        <v>84.875</v>
+        <v>79.882352941176464</v>
       </c>
     </row>
-    <row r="18" spans="1:57" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3">
         <v>2048</v>
@@ -4092,16 +4142,16 @@
         <v>0</v>
       </c>
       <c r="AQ18" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR18" s="10" t="b">
         <v>1</v>
       </c>
       <c r="AS18" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT18" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU18" s="10" t="b">
         <v>0</v>
@@ -4130,24 +4180,27 @@
       <c r="BC18" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD18" s="9">
-        <f>COUNTIF($G18:$BC18, "SYS")+COUNTIF($G18:$BC18, TRUE)</f>
-        <v>21</v>
-      </c>
-      <c r="BE18" s="4">
+      <c r="BD18" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="9">
+        <f>COUNTIF($G18:$BD18, "SYS")+COUNTIF($G18:$BD18, TRUE)</f>
+        <v>22</v>
+      </c>
+      <c r="BF18" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 18:18)/_xlfn.XLOOKUP("Feature count", $1:$1, 18:18)</f>
-        <v>97.523809523809518</v>
+        <v>93.090909090909093</v>
       </c>
     </row>
-    <row r="19" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="3">
         <v>1805</v>
@@ -4172,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L19" s="10" t="b">
         <v>1</v>
@@ -4181,13 +4234,13 @@
         <v>1</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O19" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q19" s="10" t="b">
         <v>1</v>
@@ -4265,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="AP19" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ19" s="10" t="b">
         <v>0</v>
@@ -4306,24 +4359,27 @@
       <c r="BC19" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD19" s="9">
-        <f>COUNTIF($G19:$BC19, "SYS")+COUNTIF($G19:$BC19, TRUE)</f>
-        <v>14</v>
-      </c>
-      <c r="BE19" s="4">
+      <c r="BD19" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="9">
+        <f>COUNTIF($G19:$BD19, "SYS")+COUNTIF($G19:$BD19, TRUE)</f>
+        <v>15</v>
+      </c>
+      <c r="BF19" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 19:19)/_xlfn.XLOOKUP("Feature count", $1:$1, 19:19)</f>
-        <v>128.92857142857142</v>
+        <v>120.33333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="3">
         <v>4016</v>
@@ -4354,16 +4410,16 @@
         <v>1</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O20" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q20" s="10" t="b">
         <v>1</v>
@@ -4450,10 +4506,10 @@
         <v>0</v>
       </c>
       <c r="AS20" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU20" s="10" t="b">
         <v>1</v>
@@ -4468,10 +4524,10 @@
         <v>1</v>
       </c>
       <c r="AY20" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ20" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA20" s="10" t="b">
         <v>0</v>
@@ -4482,24 +4538,27 @@
       <c r="BC20" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD20" s="9">
-        <f>COUNTIF($G20:$BC20, "SYS")+COUNTIF($G20:$BC20, TRUE)</f>
+      <c r="BD20" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="9">
+        <f>COUNTIF($G20:$BD20, "SYS")+COUNTIF($G20:$BD20, TRUE)</f>
         <v>30</v>
       </c>
-      <c r="BE20" s="4">
+      <c r="BF20" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 20:20)/_xlfn.XLOOKUP("Feature count", $1:$1, 20:20)</f>
         <v>133.86666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="3">
         <v>1896</v>
@@ -4626,13 +4685,13 @@
         <v>0</v>
       </c>
       <c r="AS21" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT21" s="10" t="b">
         <v>0</v>
       </c>
       <c r="AU21" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV21" s="10" t="b">
         <v>0</v>
@@ -4644,13 +4703,13 @@
         <v>0</v>
       </c>
       <c r="AY21" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ21" s="10" t="b">
         <v>0</v>
       </c>
       <c r="BA21" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB21" s="10" t="b">
         <v>0</v>
@@ -4658,210 +4717,216 @@
       <c r="BC21" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD21" s="9">
-        <f>COUNTIF($G21:$BC21, "SYS")+COUNTIF($G21:$BC21, TRUE)</f>
+      <c r="BD21" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="9">
+        <f>COUNTIF($G21:$BD21, "SYS")+COUNTIF($G21:$BD21, TRUE)</f>
         <v>14</v>
       </c>
-      <c r="BE21" s="4">
+      <c r="BF21" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 21:21)/_xlfn.XLOOKUP("Feature count", $1:$1, 21:21)</f>
         <v>135.42857142857142</v>
       </c>
     </row>
-    <row r="22" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3">
-        <v>2738</v>
+        <v>3998</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)+_xlfn.XLOOKUP("Extra size", $1:$1, 22:22)</f>
+        <v>3998</v>
+      </c>
+      <c r="G22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="V22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="X22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE22" s="9">
+        <f>COUNTIF($G22:$BD22, "SYS")+COUNTIF($G22:$BD22, TRUE)</f>
+        <v>25</v>
+      </c>
+      <c r="BF22" s="4">
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)/_xlfn.XLOOKUP("Feature count", $1:$1, 22:22)</f>
+        <v>159.91999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3">
         <v>2738</v>
-      </c>
-      <c r="G22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="S22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="U22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="V22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="W22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="X22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AY22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BA22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BB22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BC22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD22" s="9">
-        <f>COUNTIF($G22:$BC22, "SYS")+COUNTIF($G22:$BC22, TRUE)</f>
-        <v>18</v>
-      </c>
-      <c r="BE22" s="4">
-        <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)/_xlfn.XLOOKUP("Feature count", $1:$1, 22:22)</f>
-        <v>152.11111111111111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:57" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="3">
-        <v>3998</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
       </c>
       <c r="F23" s="3">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 23:23)+_xlfn.XLOOKUP("Extra size", $1:$1, 23:23)</f>
-        <v>3998</v>
+        <v>2738</v>
       </c>
       <c r="G23" s="10" t="b">
         <v>1</v>
@@ -4875,20 +4940,20 @@
       <c r="J23" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="K23" s="10" t="s">
-        <v>25</v>
+      <c r="K23" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="L23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="10" t="b">
         <v>0</v>
@@ -4927,19 +4992,19 @@
         <v>1</v>
       </c>
       <c r="AB23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="10" t="b">
         <v>0</v>
       </c>
       <c r="AE23" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG23" s="10" t="b">
         <v>0</v>
@@ -4966,7 +5031,7 @@
         <v>0</v>
       </c>
       <c r="AO23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP23" s="10" t="b">
         <v>0</v>
@@ -4981,10 +5046,10 @@
         <v>0</v>
       </c>
       <c r="AT23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV23" s="10" t="b">
         <v>0</v>
@@ -4999,10 +5064,10 @@
         <v>0</v>
       </c>
       <c r="AZ23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB23" s="10" t="b">
         <v>0</v>
@@ -5010,24 +5075,27 @@
       <c r="BC23" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD23" s="9">
-        <f>COUNTIF($G23:$BC23, "SYS")+COUNTIF($G23:$BC23, TRUE)</f>
-        <v>25</v>
-      </c>
-      <c r="BE23" s="4">
+      <c r="BD23" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE23" s="9">
+        <f>COUNTIF($G23:$BD23, "SYS")+COUNTIF($G23:$BD23, TRUE)</f>
+        <v>17</v>
+      </c>
+      <c r="BF23" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 23:23)/_xlfn.XLOOKUP("Feature count", $1:$1, 23:23)</f>
-        <v>159.91999999999999</v>
+        <v>161.05882352941177</v>
       </c>
     </row>
-    <row r="24" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="3">
         <v>2824</v>
@@ -5186,34 +5254,37 @@
       <c r="BC24" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD24" s="9">
-        <f>COUNTIF($G24:$BC24, "SYS")+COUNTIF($G24:$BC24, TRUE)</f>
+      <c r="BD24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE24" s="9">
+        <f>COUNTIF($G24:$BD24, "SYS")+COUNTIF($G24:$BD24, TRUE)</f>
         <v>17</v>
       </c>
-      <c r="BE24" s="4">
+      <c r="BF24" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 24:24)/_xlfn.XLOOKUP("Feature count", $1:$1, 24:24)</f>
         <v>166.11764705882354</v>
       </c>
     </row>
-    <row r="25" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3">
-        <v>2710</v>
+        <v>2882</v>
       </c>
       <c r="E25" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 25:25)+_xlfn.XLOOKUP("Extra size", $1:$1, 25:25)</f>
-        <v>2810</v>
+        <v>2882</v>
       </c>
       <c r="G25" s="10" t="b">
         <v>1</v>
@@ -5228,22 +5299,22 @@
         <v>1</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L25" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="M25" s="10" t="s">
-        <v>25</v>
+      <c r="M25" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O25" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="P25" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="Q25" s="10" t="b">
         <v>1</v>
@@ -5255,13 +5326,13 @@
         <v>1</v>
       </c>
       <c r="T25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="10" t="b">
         <v>0</v>
@@ -5276,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="AA25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB25" s="10" t="b">
         <v>0</v>
@@ -5288,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="AE25" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF25" s="10" t="b">
         <v>0</v>
@@ -5330,7 +5401,7 @@
         <v>0</v>
       </c>
       <c r="AS25" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT25" s="10" t="b">
         <v>0</v>
@@ -5362,210 +5433,216 @@
       <c r="BC25" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="BD25" s="9">
-        <f>COUNTIF($G25:$BC25, "SYS")+COUNTIF($G25:$BC25, TRUE)</f>
+      <c r="BD25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE25" s="9">
+        <f>COUNTIF($G25:$BD25, "SYS")+COUNTIF($G25:$BD25, TRUE)</f>
         <v>16</v>
       </c>
-      <c r="BE25" s="4">
+      <c r="BF25" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 25:25)/_xlfn.XLOOKUP("Feature count", $1:$1, 25:25)</f>
-        <v>169.375</v>
+        <v>180.125</v>
       </c>
     </row>
-    <row r="26" spans="1:57" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D26" s="3">
-        <v>4095</v>
+        <v>2710</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F26" s="3">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)+_xlfn.XLOOKUP("Extra size", $1:$1, 26:26)</f>
+        <v>2810</v>
+      </c>
+      <c r="G26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="U26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="V26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="W26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="X26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE26" s="9">
+        <f>COUNTIF($G26:$BD26, "SYS")+COUNTIF($G26:$BD26, TRUE)</f>
+        <v>15</v>
+      </c>
+      <c r="BF26" s="4">
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)/_xlfn.XLOOKUP("Feature count", $1:$1, 26:26)</f>
+        <v>180.66666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:58" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="3">
         <v>4095</v>
-      </c>
-      <c r="G26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="S26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="U26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="V26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="W26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="X26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AY26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BB26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD26" s="9">
-        <f>COUNTIF($G26:$BC26, "SYS")+COUNTIF($G26:$BC26, TRUE)</f>
-        <v>23</v>
-      </c>
-      <c r="BE26" s="4">
-        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)/_xlfn.XLOOKUP("Feature count", $1:$1, 26:26)</f>
-        <v>178.04347826086956</v>
-      </c>
-    </row>
-    <row r="27" spans="1:57" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="3">
-        <v>2882</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)+_xlfn.XLOOKUP("Extra size", $1:$1, 27:27)</f>
-        <v>2882</v>
+        <v>4095</v>
       </c>
       <c r="G27" s="10" t="b">
         <v>1</v>
@@ -5580,7 +5657,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L27" s="10" t="b">
         <v>1</v>
@@ -5589,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O27" s="10" t="b">
         <v>0</v>
@@ -5637,7 +5714,7 @@
         <v>0</v>
       </c>
       <c r="AD27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE27" s="10" t="b">
         <v>0</v>
@@ -5646,10 +5723,10 @@
         <v>0</v>
       </c>
       <c r="AG27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI27" s="10" t="b">
         <v>0</v>
@@ -5697,7 +5774,7 @@
         <v>0</v>
       </c>
       <c r="AX27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY27" s="10" t="b">
         <v>0</v>
@@ -5706,32 +5783,35 @@
         <v>0</v>
       </c>
       <c r="BA27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB27" s="10" t="b">
         <v>0</v>
       </c>
       <c r="BC27" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD27" s="9">
-        <f>COUNTIF($G27:$BC27, "SYS")+COUNTIF($G27:$BC27, TRUE)</f>
-        <v>16</v>
-      </c>
-      <c r="BE27" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD27" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE27" s="9">
+        <f>COUNTIF($G27:$BD27, "SYS")+COUNTIF($G27:$BD27, TRUE)</f>
+        <v>22</v>
+      </c>
+      <c r="BF27" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)/_xlfn.XLOOKUP("Feature count", $1:$1, 27:27)</f>
-        <v>180.125</v>
+        <v>186.13636363636363</v>
       </c>
     </row>
-    <row r="28" spans="1:57" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:58" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D28" s="3">
         <v>4002</v>
@@ -5765,7 +5845,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O28" s="10" t="b">
         <v>1</v>
@@ -5849,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="AP28" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ28" s="10" t="b">
         <v>0</v>
@@ -5879,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="AZ28" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA28" s="10" t="b">
         <v>0</v>
@@ -5888,21 +5968,24 @@
         <v>0</v>
       </c>
       <c r="BC28" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD28" s="9">
-        <f>COUNTIF($G28:$BC28, "SYS")+COUNTIF($G28:$BC28, TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="BD28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BE28" s="9">
+        <f>COUNTIF($G28:$BD28, "SYS")+COUNTIF($G28:$BD28, TRUE)</f>
         <v>21</v>
       </c>
-      <c r="BE28" s="4">
+      <c r="BF28" s="4">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 28:28)/_xlfn.XLOOKUP("Feature count", $1:$1, 28:28)</f>
         <v>190.57142857142858</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BE28" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BE28">
-      <sortCondition ref="BE2:BE28"/>
+  <autoFilter ref="A2:BF28" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BF28">
+      <sortCondition ref="BF2:BF28"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5941,7 +6024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:BC28">
+  <conditionalFormatting sqref="G3:BD28">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -5952,7 +6035,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD3:BD28">
+  <conditionalFormatting sqref="BE3:BE28">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -5962,7 +6045,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE3:BE28">
+  <conditionalFormatting sqref="BF3:BF28">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -5973,31 +6056,32 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{76EB020E-CC71-B148-9424-BB7A1349A5E9}"/>
-    <hyperlink ref="A8" r:id="rId2" xr:uid="{022DC04F-D95A-7246-8451-7C3BA522CD1C}"/>
-    <hyperlink ref="A14" r:id="rId3" xr:uid="{8B9F4BC6-14C6-4345-BA9C-9D9C8BC6C54A}"/>
-    <hyperlink ref="A21" r:id="rId4" xr:uid="{1A073B5B-BE69-9E43-BB31-2AC1F74931C7}"/>
-    <hyperlink ref="A3" r:id="rId5" xr:uid="{469B8618-6944-6746-99BB-8FB17F692A90}"/>
-    <hyperlink ref="A5" r:id="rId6" xr:uid="{D6CABB3D-301E-5A48-8390-5B6D8D98891E}"/>
-    <hyperlink ref="A6" r:id="rId7" xr:uid="{1EAE54DC-A089-B24E-A04A-825543C48D1A}"/>
-    <hyperlink ref="A13" r:id="rId8" xr:uid="{65802411-1B8E-064F-A6D7-DAD404DC6F66}"/>
-    <hyperlink ref="A19" r:id="rId9" xr:uid="{B15F6BAD-35BC-2A4D-A9F9-E3397D6C9F57}"/>
-    <hyperlink ref="A20" r:id="rId10" xr:uid="{A76D4E5E-9C61-C846-BF68-39EA20E19271}"/>
-    <hyperlink ref="A25" r:id="rId11" xr:uid="{271A3F43-6A28-9044-9B77-55CB67E8E604}"/>
-    <hyperlink ref="A27" r:id="rId12" xr:uid="{3319FE9B-1572-7B45-A51A-8631F49908F5}"/>
-    <hyperlink ref="A22" r:id="rId13" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
-    <hyperlink ref="A10" r:id="rId14" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
-    <hyperlink ref="A24" r:id="rId15" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
-    <hyperlink ref="A26" r:id="rId16" xr:uid="{BE81C522-7811-534B-B250-C27D6ED80E13}"/>
+    <hyperlink ref="A14" r:id="rId1" xr:uid="{8B9F4BC6-14C6-4345-BA9C-9D9C8BC6C54A}"/>
+    <hyperlink ref="A19" r:id="rId2" xr:uid="{B15F6BAD-35BC-2A4D-A9F9-E3397D6C9F57}"/>
+    <hyperlink ref="A20" r:id="rId3" xr:uid="{A76D4E5E-9C61-C846-BF68-39EA20E19271}"/>
+    <hyperlink ref="A26" r:id="rId4" xr:uid="{271A3F43-6A28-9044-9B77-55CB67E8E604}"/>
+    <hyperlink ref="A25" r:id="rId5" xr:uid="{3319FE9B-1572-7B45-A51A-8631F49908F5}"/>
+    <hyperlink ref="A23" r:id="rId6" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
+    <hyperlink ref="A24" r:id="rId7" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
+    <hyperlink ref="A27" r:id="rId8" xr:uid="{BE81C522-7811-534B-B250-C27D6ED80E13}"/>
+    <hyperlink ref="A18" r:id="rId9" xr:uid="{7A0C5CE4-FDBB-C142-89E0-609051079143}"/>
+    <hyperlink ref="A22" r:id="rId10" xr:uid="{B27A7A0A-1947-624B-A135-AC2E4FA9DCDF}"/>
+    <hyperlink ref="A15" r:id="rId11" xr:uid="{BBFDB1C2-F4D5-9F4F-9AB4-84F69F8E341F}"/>
+    <hyperlink ref="A16" r:id="rId12" xr:uid="{47C1315B-4443-9B43-9DB9-33643DFA677C}"/>
+    <hyperlink ref="A17" r:id="rId13" xr:uid="{C77570FF-B176-1F4E-AC94-8C167340C676}"/>
+    <hyperlink ref="A21" r:id="rId14" xr:uid="{1A073B5B-BE69-9E43-BB31-2AC1F74931C7}"/>
+    <hyperlink ref="A13" r:id="rId15" xr:uid="{65802411-1B8E-064F-A6D7-DAD404DC6F66}"/>
+    <hyperlink ref="A12" r:id="rId16" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>
     <hyperlink ref="A11" r:id="rId17" xr:uid="{F2854865-7589-3148-9BD0-694117F0C02A}"/>
-    <hyperlink ref="A18" r:id="rId18" xr:uid="{7A0C5CE4-FDBB-C142-89E0-609051079143}"/>
-    <hyperlink ref="A23" r:id="rId19" xr:uid="{B27A7A0A-1947-624B-A135-AC2E4FA9DCDF}"/>
-    <hyperlink ref="A7" r:id="rId20" xr:uid="{0C291FB0-BA8C-E141-98A4-91A6B6DD9884}"/>
-    <hyperlink ref="A9" r:id="rId21" xr:uid="{2F1BE129-94F7-DB45-B74A-D5DECFC8BD1F}"/>
-    <hyperlink ref="A12" r:id="rId22" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>
-    <hyperlink ref="A15" r:id="rId23" xr:uid="{BBFDB1C2-F4D5-9F4F-9AB4-84F69F8E341F}"/>
-    <hyperlink ref="A16" r:id="rId24" xr:uid="{47C1315B-4443-9B43-9DB9-33643DFA677C}"/>
-    <hyperlink ref="A17" r:id="rId25" xr:uid="{C77570FF-B176-1F4E-AC94-8C167340C676}"/>
+    <hyperlink ref="A10" r:id="rId18" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
+    <hyperlink ref="A9" r:id="rId19" xr:uid="{2F1BE129-94F7-DB45-B74A-D5DECFC8BD1F}"/>
+    <hyperlink ref="A8" r:id="rId20" xr:uid="{022DC04F-D95A-7246-8451-7C3BA522CD1C}"/>
+    <hyperlink ref="A7" r:id="rId21" xr:uid="{0C291FB0-BA8C-E141-98A4-91A6B6DD9884}"/>
+    <hyperlink ref="A6" r:id="rId22" xr:uid="{1EAE54DC-A089-B24E-A04A-825543C48D1A}"/>
+    <hyperlink ref="A5" r:id="rId23" xr:uid="{D6CABB3D-301E-5A48-8390-5B6D8D98891E}"/>
+    <hyperlink ref="A4" r:id="rId24" xr:uid="{76EB020E-CC71-B148-9424-BB7A1349A5E9}"/>
+    <hyperlink ref="A3" r:id="rId25" xr:uid="{469B8618-6944-6746-99BB-8FB17F692A90}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{D7B84B32-63C9-7A46-AF5A-77D30F18AB91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
persistent high scores + note
</commit_message>
<xml_diff>
--- a/tetris-4k-archive.xlsx
+++ b/tetris-4k-archive.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493d989091475df7/Personal/GitHub/tetris4karchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1339" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E239A2B-D2DB-6F47-9311-12763238ED2F}"/>
+  <xr:revisionPtr revIDLastSave="1430" documentId="8_{0CDAABD7-AF78-CC49-9CC2-90DD68763645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D49A92B7-5207-184A-9B37-F62B76D6EE7C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21140" xr2:uid="{F4EAB821-2EDC-3446-8812-752F41EB9B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$BH$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$BI$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
   <si>
     <t>Url</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>No ceiling</t>
+  </si>
+  <si>
+    <t>Persistent high scores</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -582,9 +585,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -950,11 +952,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
-  <dimension ref="A1:BI31"/>
+  <dimension ref="A1:BJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL33" sqref="AL33"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,12 +967,16 @@
     <col min="4" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="19" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.6640625" customWidth="1"/>
-    <col min="21" max="59" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="111" width="10.83203125" customWidth="1"/>
+    <col min="21" max="27" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.6640625" customWidth="1"/>
+    <col min="29" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="3.6640625" customWidth="1"/>
+    <col min="39" max="60" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="112" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1080,360 +1086,368 @@
         <v>63</v>
       </c>
       <c r="AK1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL1" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AM1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AN1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AO1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AP1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AR1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AS1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AT1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AU1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AV1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AW1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="AW1" s="7" t="s">
+      <c r="AX1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="AY1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AZ1" s="7" t="s">
+      <c r="BA1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BB1" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BC1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BD1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BE1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BF1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BG1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BH1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BI1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
     </row>
-    <row r="2" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12">
         <f>COUNTIF(G$4:G$31, "&gt;0")</f>
         <v>27</v>
       </c>
-      <c r="H2" s="13">
-        <f t="shared" ref="H2:BF2" si="0">COUNTIF(H$4:H$31, "&gt;0")</f>
+      <c r="H2" s="12">
+        <f t="shared" ref="H2:BG2" si="0">COUNTIF(H$4:H$31, "&gt;0")</f>
         <v>27</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="12">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="12">
         <f>COUNTIF(T$4:T$31, "&gt;0")</f>
         <v>6</v>
       </c>
-      <c r="U2" s="13">
+      <c r="U2" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="W2" s="13">
-        <f t="shared" si="0"/>
+      <c r="W2" s="12">
+        <f>COUNTIF(W$4:W$31, "&gt;0")</f>
         <v>16</v>
       </c>
-      <c r="X2" s="13">
-        <f t="shared" si="0"/>
+      <c r="X2" s="12">
+        <f>COUNTIF(X$4:X$31, "&gt;0")</f>
         <v>13</v>
       </c>
-      <c r="Y2" s="13">
-        <f t="shared" si="0"/>
+      <c r="Y2" s="12">
+        <f>COUNTIF(Y$4:Y$31, "&gt;0")</f>
         <v>13</v>
       </c>
-      <c r="Z2" s="13">
-        <f t="shared" si="0"/>
+      <c r="Z2" s="12">
+        <f>COUNTIF(Z$4:Z$31, "&gt;0")</f>
         <v>12</v>
       </c>
-      <c r="AA2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AA2" s="12">
+        <f>COUNTIF(AA$4:AA$31, "&gt;0")</f>
         <v>6</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AB2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AC2" s="13">
+      <c r="AC2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AD2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AD2" s="12">
+        <f>COUNTIF(AD$4:AD$31, "&gt;0")</f>
         <v>21</v>
       </c>
-      <c r="AE2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AE2" s="12">
+        <f>COUNTIF(AE$4:AE$31, "&gt;0")</f>
         <v>15</v>
       </c>
-      <c r="AF2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AF2" s="12">
+        <f>COUNTIF(AF$4:AF$31, "&gt;0")</f>
         <v>16</v>
       </c>
-      <c r="AG2" s="13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="AH2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AG2" s="12">
+        <f>COUNTIF(AG$4:AG$31, "&gt;0")</f>
         <v>5</v>
       </c>
-      <c r="AI2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AH2" s="12">
+        <f>COUNTIF(AH$4:AH$31, "&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="AI2" s="12">
+        <f>COUNTIF(AI$4:AI$31, "&gt;0")</f>
         <v>4</v>
       </c>
-      <c r="AJ2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AJ2" s="12">
+        <f>COUNTIF(AJ$4:AJ$31, "&gt;0")</f>
         <v>4</v>
       </c>
-      <c r="AK2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AL2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AM2" s="13">
+      <c r="AK2" s="12">
+        <f>COUNTIF(AK$4:AK$31, "&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="AL2" s="12">
+        <f>COUNTIF(AL$4:AL$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="AM2" s="12">
+        <f>COUNTIF(AM$4:AM$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="AN2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AN2" s="13">
+      <c r="AO2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AO2" s="13">
+      <c r="AP2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AP2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AQ2" s="12">
+        <f>COUNTIF(AQ$4:AQ$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="AR2" s="12">
+        <f>COUNTIF(AR$4:AR$31, "&gt;0")</f>
         <v>3</v>
       </c>
-      <c r="AR2" s="13">
-        <f t="shared" si="0"/>
+      <c r="AS2" s="12">
+        <f>COUNTIF(AS$4:AS$31, "&gt;0")</f>
         <v>4</v>
       </c>
-      <c r="AS2" s="13">
+      <c r="AT2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AT2" s="13">
+      <c r="AU2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AU2" s="13">
+      <c r="AV2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AV2" s="13">
+      <c r="AW2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AW2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AX2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AY2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AZ2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="BA2" s="13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="BB2" s="13">
+      <c r="AX2" s="12">
+        <f>COUNTIF(AX$4:AX$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="AY2" s="12">
+        <f>COUNTIF(AY$4:AY$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="AZ2" s="12">
+        <f>COUNTIF(AZ$4:AZ$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="BA2" s="12">
+        <f>COUNTIF(BA$4:BA$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="BB2" s="12">
+        <f>COUNTIF(BB$4:BB$31, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="BC2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BC2" s="13">
+      <c r="BD2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BD2" s="13">
+      <c r="BE2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BE2" s="13">
+      <c r="BF2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BF2" s="13">
+      <c r="BG2" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BG2" s="13"/>
-      <c r="BH2" s="13"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="12"/>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="12"/>
-      <c r="AY3" s="12"/>
-      <c r="AZ3" s="12"/>
-      <c r="BA3" s="12"/>
-      <c r="BB3" s="12"/>
-      <c r="BC3" s="12"/>
-      <c r="BD3" s="12"/>
-      <c r="BE3" s="12"/>
-      <c r="BF3" s="12"/>
-      <c r="BG3" s="12"/>
-      <c r="BH3" s="12"/>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="11"/>
+      <c r="AW3" s="11"/>
+      <c r="AX3" s="11"/>
+      <c r="AY3" s="11"/>
+      <c r="AZ3" s="11"/>
+      <c r="BA3" s="11"/>
+      <c r="BB3" s="11"/>
+      <c r="BC3" s="11"/>
+      <c r="BD3" s="11"/>
+      <c r="BE3" s="11"/>
+      <c r="BF3" s="11"/>
+      <c r="BG3" s="11"/>
+      <c r="BH3" s="11"/>
+      <c r="BI3" s="11"/>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>108</v>
       </c>
@@ -1609,16 +1623,19 @@
       <c r="BF4" s="4">
         <v>0</v>
       </c>
-      <c r="BG4" s="6">
-        <f>COUNTIF($G4:$BF4, "&gt;0")</f>
+      <c r="BG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH4" s="6">
+        <f>COUNTIF($G4:$BG4, "&gt;0")</f>
         <v>16</v>
       </c>
-      <c r="BH4" s="10">
+      <c r="BI4" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 4:4)/_xlfn.XLOOKUP("Feature count", $1:$1, 4:4)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>91</v>
       </c>
@@ -1794,16 +1811,19 @@
       <c r="BF5" s="4">
         <v>0</v>
       </c>
-      <c r="BG5" s="6">
-        <f>COUNTIF($G5:$BF5, "&gt;0")</f>
+      <c r="BG5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="6">
+        <f>COUNTIF($G5:$BG5, "&gt;0")</f>
         <v>17</v>
       </c>
-      <c r="BH5" s="10">
+      <c r="BI5" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 5:5)/_xlfn.XLOOKUP("Feature count", $1:$1, 5:5)</f>
         <v>29.882352941176471</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>75</v>
       </c>
@@ -1979,16 +1999,19 @@
       <c r="BF6" s="4">
         <v>0</v>
       </c>
-      <c r="BG6" s="6">
-        <f>COUNTIF($G6:$BF6, "&gt;0")</f>
+      <c r="BG6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="6">
+        <f>COUNTIF($G6:$BG6, "&gt;0")</f>
         <v>10</v>
       </c>
-      <c r="BH6" s="10">
+      <c r="BI6" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 6:6)/_xlfn.XLOOKUP("Feature count", $1:$1, 6:6)</f>
         <v>30.4</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>107</v>
       </c>
@@ -2164,16 +2187,19 @@
       <c r="BF7" s="4">
         <v>0</v>
       </c>
-      <c r="BG7" s="6">
-        <f>COUNTIF($G7:$BF7, "&gt;0")</f>
+      <c r="BG7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="6">
+        <f>COUNTIF($G7:$BG7, "&gt;0")</f>
         <v>8</v>
       </c>
-      <c r="BH7" s="10">
+      <c r="BI7" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 7:7)/_xlfn.XLOOKUP("Feature count", $1:$1, 7:7)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>76</v>
       </c>
@@ -2349,16 +2375,19 @@
       <c r="BF8" s="4">
         <v>0</v>
       </c>
-      <c r="BG8" s="6">
-        <f>COUNTIF($G8:$BF8, "&gt;0")</f>
+      <c r="BG8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="6">
+        <f>COUNTIF($G8:$BG8, "&gt;0")</f>
         <v>14</v>
       </c>
-      <c r="BH8" s="10">
+      <c r="BI8" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 8:8)/_xlfn.XLOOKUP("Feature count", $1:$1, 8:8)</f>
         <v>33.142857142857146</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>85</v>
       </c>
@@ -2534,16 +2563,19 @@
       <c r="BF9" s="4">
         <v>0</v>
       </c>
-      <c r="BG9" s="6">
-        <f>COUNTIF($G9:$BF9, "&gt;0")</f>
+      <c r="BG9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="6">
+        <f>COUNTIF($G9:$BG9, "&gt;0")</f>
         <v>14</v>
       </c>
-      <c r="BH9" s="10">
+      <c r="BI9" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 9:9)/_xlfn.XLOOKUP("Feature count", $1:$1, 9:9)</f>
         <v>33.642857142857146</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>77</v>
       </c>
@@ -2719,16 +2751,19 @@
       <c r="BF10" s="4">
         <v>0</v>
       </c>
-      <c r="BG10" s="6">
-        <f>COUNTIF($G10:$BF10, "&gt;0")</f>
+      <c r="BG10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="6">
+        <f>COUNTIF($G10:$BG10, "&gt;0")</f>
         <v>8</v>
       </c>
-      <c r="BH10" s="10">
+      <c r="BI10" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 10:10)/_xlfn.XLOOKUP("Feature count", $1:$1, 10:10)</f>
         <v>34.25</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>78</v>
       </c>
@@ -2904,16 +2939,19 @@
       <c r="BF11" s="4">
         <v>0</v>
       </c>
-      <c r="BG11" s="6">
-        <f>COUNTIF($G11:$BF11, "&gt;0")</f>
+      <c r="BG11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH11" s="6">
+        <f>COUNTIF($G11:$BG11, "&gt;0")</f>
         <v>7</v>
       </c>
-      <c r="BH11" s="10">
+      <c r="BI11" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 11:11)/_xlfn.XLOOKUP("Feature count", $1:$1, 11:11)</f>
         <v>35.857142857142854</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>80</v>
       </c>
@@ -3089,219 +3127,225 @@
       <c r="BF12" s="4">
         <v>0</v>
       </c>
-      <c r="BG12" s="6">
-        <f>COUNTIF($G12:$BF12, "&gt;0")</f>
+      <c r="BG12" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH12" s="6">
+        <f>COUNTIF($G12:$BG12, "&gt;0")</f>
         <v>10</v>
       </c>
-      <c r="BH12" s="10">
+      <c r="BI12" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 12:12)/_xlfn.XLOOKUP("Feature count", $1:$1, 12:12)</f>
         <v>44.6</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="9">
-        <v>510</v>
+        <v>1459</v>
       </c>
       <c r="E13" s="9">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="F13" s="9">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)+_xlfn.XLOOKUP("Extra size", $1:$1, 13:13)</f>
+        <v>1550</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2</v>
+      </c>
+      <c r="M13" s="4">
+        <v>2</v>
+      </c>
+      <c r="N13" s="4">
+        <v>2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <v>2</v>
+      </c>
+      <c r="S13" s="4">
+        <v>2</v>
+      </c>
+      <c r="T13" s="4">
+        <v>2</v>
+      </c>
+      <c r="U13" s="4">
+        <v>2</v>
+      </c>
+      <c r="V13" s="4">
+        <v>2</v>
+      </c>
+      <c r="W13" s="4">
+        <v>2</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AO13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AP13" s="4">
+        <v>2</v>
+      </c>
+      <c r="AQ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG13" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH13" s="6">
+        <f>COUNTIF($G13:$BG13, "&gt;0")</f>
+        <v>32</v>
+      </c>
+      <c r="BI13" s="10">
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)/_xlfn.XLOOKUP("Feature count", $1:$1, 13:13)</f>
+        <v>45.59375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
         <v>510</v>
       </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2</v>
-      </c>
-      <c r="I13" s="4">
-        <v>2</v>
-      </c>
-      <c r="J13" s="4">
-        <v>2</v>
-      </c>
-      <c r="K13" s="4">
-        <v>2</v>
-      </c>
-      <c r="L13" s="4">
-        <v>2</v>
-      </c>
-      <c r="M13" s="4">
-        <v>2</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>2</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
-        <v>0</v>
-      </c>
-      <c r="U13" s="4">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4">
-        <v>0</v>
-      </c>
-      <c r="W13" s="4">
-        <v>0</v>
-      </c>
-      <c r="X13" s="4">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BE13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BF13" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG13" s="6">
-        <f>COUNTIF($G13:$BF13, "&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="BH13" s="10">
-        <f>_xlfn.XLOOKUP("Main size", $1:$1, 13:13)/_xlfn.XLOOKUP("Feature count", $1:$1, 13:13)</f>
-        <v>46.363636363636367</v>
-      </c>
-    </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1459</v>
-      </c>
       <c r="E14" s="9">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="F14" s="9">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 14:14)+_xlfn.XLOOKUP("Extra size", $1:$1, 14:14)</f>
-        <v>1550</v>
+        <v>510</v>
       </c>
       <c r="G14" s="4">
         <v>2</v>
@@ -3325,46 +3369,46 @@
         <v>2</v>
       </c>
       <c r="N14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X14" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="4">
         <v>0</v>
@@ -3376,37 +3420,37 @@
         <v>2</v>
       </c>
       <c r="AE14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP14" s="4">
         <v>0</v>
@@ -3459,16 +3503,19 @@
       <c r="BF14" s="4">
         <v>0</v>
       </c>
-      <c r="BG14" s="6">
-        <f>COUNTIF($G14:$BF14, "&gt;0")</f>
-        <v>31</v>
-      </c>
-      <c r="BH14" s="10">
+      <c r="BG14" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH14" s="6">
+        <f>COUNTIF($G14:$BG14, "&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="BI14" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 14:14)/_xlfn.XLOOKUP("Feature count", $1:$1, 14:14)</f>
-        <v>47.064516129032256</v>
+        <v>46.363636363636367</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
@@ -3594,10 +3641,10 @@
         <v>0</v>
       </c>
       <c r="AP15" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR15" s="4">
         <v>0</v>
@@ -3644,16 +3691,19 @@
       <c r="BF15" s="4">
         <v>0</v>
       </c>
-      <c r="BG15" s="6">
-        <f>COUNTIF($G15:$BF15, "&gt;0")</f>
+      <c r="BG15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH15" s="6">
+        <f>COUNTIF($G15:$BG15, "&gt;0")</f>
         <v>10</v>
       </c>
-      <c r="BH15" s="10">
+      <c r="BI15" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 15:15)/_xlfn.XLOOKUP("Feature count", $1:$1, 15:15)</f>
         <v>49.1</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>87</v>
       </c>
@@ -3779,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="AP16" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR16" s="4">
         <v>0</v>
@@ -3829,16 +3879,19 @@
       <c r="BF16" s="4">
         <v>0</v>
       </c>
-      <c r="BG16" s="6">
-        <f>COUNTIF($G16:$BF16, "&gt;0")</f>
+      <c r="BG16" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH16" s="6">
+        <f>COUNTIF($G16:$BG16, "&gt;0")</f>
         <v>8</v>
       </c>
-      <c r="BH16" s="10">
+      <c r="BI16" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 16:16)/_xlfn.XLOOKUP("Feature count", $1:$1, 16:16)</f>
         <v>55.75</v>
       </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>86</v>
       </c>
@@ -3967,10 +4020,10 @@
         <v>0</v>
       </c>
       <c r="AQ17" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR17" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS17" s="4">
         <v>0</v>
@@ -4014,16 +4067,19 @@
       <c r="BF17" s="4">
         <v>0</v>
       </c>
-      <c r="BG17" s="6">
-        <f>COUNTIF($G17:$BF17, "&gt;0")</f>
+      <c r="BG17" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH17" s="6">
+        <f>COUNTIF($G17:$BG17, "&gt;0")</f>
         <v>4</v>
       </c>
-      <c r="BH17" s="10">
+      <c r="BI17" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 17:17)/_xlfn.XLOOKUP("Feature count", $1:$1, 17:17)</f>
         <v>56.75</v>
       </c>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>88</v>
       </c>
@@ -4199,16 +4255,19 @@
       <c r="BF18" s="4">
         <v>0</v>
       </c>
-      <c r="BG18" s="6">
-        <f>COUNTIF($G18:$BF18, "&gt;0")</f>
+      <c r="BG18" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH18" s="6">
+        <f>COUNTIF($G18:$BG18, "&gt;0")</f>
         <v>7</v>
       </c>
-      <c r="BH18" s="10">
+      <c r="BI18" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 18:18)/_xlfn.XLOOKUP("Feature count", $1:$1, 18:18)</f>
         <v>65.285714285714292</v>
       </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>89</v>
       </c>
@@ -4384,16 +4443,19 @@
       <c r="BF19" s="4">
         <v>0</v>
       </c>
-      <c r="BG19" s="6">
-        <f>COUNTIF($G19:$BF19, "&gt;0")</f>
+      <c r="BG19" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="6">
+        <f>COUNTIF($G19:$BG19, "&gt;0")</f>
         <v>18</v>
       </c>
-      <c r="BH19" s="10">
+      <c r="BI19" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 19:19)/_xlfn.XLOOKUP("Feature count", $1:$1, 19:19)</f>
         <v>70.5</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>90</v>
       </c>
@@ -4525,13 +4587,13 @@
         <v>0</v>
       </c>
       <c r="AR20" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS20" s="4">
         <v>2</v>
       </c>
       <c r="AT20" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU20" s="4">
         <v>0</v>
@@ -4569,16 +4631,19 @@
       <c r="BF20" s="4">
         <v>0</v>
       </c>
-      <c r="BG20" s="6">
-        <f>COUNTIF($G20:$BF20, "&gt;0")</f>
+      <c r="BG20" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH20" s="6">
+        <f>COUNTIF($G20:$BG20, "&gt;0")</f>
         <v>18</v>
       </c>
-      <c r="BH20" s="10">
+      <c r="BI20" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 20:20)/_xlfn.XLOOKUP("Feature count", $1:$1, 20:20)</f>
         <v>75.444444444444443</v>
       </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>92</v>
       </c>
@@ -4677,7 +4742,7 @@
         <v>2</v>
       </c>
       <c r="AG21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH21" s="4">
         <v>0</v>
@@ -4716,7 +4781,7 @@
         <v>0</v>
       </c>
       <c r="AT21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU21" s="4">
         <v>2</v>
@@ -4725,7 +4790,7 @@
         <v>2</v>
       </c>
       <c r="AW21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX21" s="4">
         <v>0</v>
@@ -4754,16 +4819,19 @@
       <c r="BF21" s="4">
         <v>0</v>
       </c>
-      <c r="BG21" s="6">
-        <f>COUNTIF($G21:$BF21, "&gt;0")</f>
-        <v>22</v>
-      </c>
-      <c r="BH21" s="10">
+      <c r="BG21" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH21" s="6">
+        <f>COUNTIF($G21:$BG21, "&gt;0")</f>
+        <v>21</v>
+      </c>
+      <c r="BI21" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 21:21)/_xlfn.XLOOKUP("Feature count", $1:$1, 21:21)</f>
-        <v>93.090909090909093</v>
+        <v>97.523809523809518</v>
       </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>98</v>
       </c>
@@ -4910,13 +4978,13 @@
         <v>0</v>
       </c>
       <c r="AW22" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX22" s="4">
         <v>2</v>
       </c>
       <c r="AY22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ22" s="4">
         <v>0</v>
@@ -4939,16 +5007,19 @@
       <c r="BF22" s="4">
         <v>0</v>
       </c>
-      <c r="BG22" s="6">
-        <f>COUNTIF($G22:$BF22, "&gt;0")</f>
+      <c r="BG22" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH22" s="6">
+        <f>COUNTIF($G22:$BG22, "&gt;0")</f>
         <v>16</v>
       </c>
-      <c r="BH22" s="10">
+      <c r="BI22" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 22:22)/_xlfn.XLOOKUP("Feature count", $1:$1, 22:22)</f>
         <v>118.5</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>96</v>
       </c>
@@ -5080,10 +5151,10 @@
         <v>0</v>
       </c>
       <c r="AR23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS23" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT23" s="4">
         <v>0</v>
@@ -5124,16 +5195,19 @@
       <c r="BF23" s="4">
         <v>0</v>
       </c>
-      <c r="BG23" s="6">
-        <f>COUNTIF($G23:$BF23, "&gt;0")</f>
+      <c r="BG23" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH23" s="6">
+        <f>COUNTIF($G23:$BG23, "&gt;0")</f>
         <v>15</v>
       </c>
-      <c r="BH23" s="10">
+      <c r="BI23" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 23:23)/_xlfn.XLOOKUP("Feature count", $1:$1, 23:23)</f>
         <v>120.33333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>97</v>
       </c>
@@ -5244,13 +5318,13 @@
         <v>2</v>
       </c>
       <c r="AK24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL24" s="4">
         <v>2</v>
       </c>
       <c r="AM24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN24" s="4">
         <v>0</v>
@@ -5262,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="AQ24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS24" s="4">
         <v>0</v>
@@ -5280,13 +5354,13 @@
         <v>0</v>
       </c>
       <c r="AW24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ24" s="4">
         <v>2</v>
@@ -5301,7 +5375,7 @@
         <v>2</v>
       </c>
       <c r="BD24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE24" s="4">
         <v>0</v>
@@ -5309,16 +5383,19 @@
       <c r="BF24" s="4">
         <v>0</v>
       </c>
-      <c r="BG24" s="6">
-        <f>COUNTIF($G24:$BF24, "&gt;0")</f>
+      <c r="BG24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH24" s="6">
+        <f>COUNTIF($G24:$BG24, "&gt;0")</f>
         <v>31</v>
       </c>
-      <c r="BH24" s="10">
+      <c r="BI24" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 24:24)/_xlfn.XLOOKUP("Feature count", $1:$1, 24:24)</f>
         <v>129.54838709677421</v>
       </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>99</v>
       </c>
@@ -5447,13 +5524,13 @@
         <v>0</v>
       </c>
       <c r="AQ25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR25" s="4">
         <v>2</v>
       </c>
       <c r="AS25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT25" s="4">
         <v>0</v>
@@ -5471,13 +5548,13 @@
         <v>0</v>
       </c>
       <c r="AY25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ25" s="4">
         <v>2</v>
       </c>
       <c r="BA25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB25" s="4">
         <v>0</v>
@@ -5486,227 +5563,233 @@
         <v>0</v>
       </c>
       <c r="BD25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF25" s="4">
         <v>0</v>
       </c>
-      <c r="BG25" s="6">
-        <f>COUNTIF($G25:$BF25, "&gt;0")</f>
+      <c r="BG25" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH25" s="6">
+        <f>COUNTIF($G25:$BG25, "&gt;0")</f>
         <v>26</v>
       </c>
-      <c r="BH25" s="10">
+      <c r="BI25" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 25:25)/_xlfn.XLOOKUP("Feature count", $1:$1, 25:25)</f>
         <v>153.76923076923077</v>
       </c>
     </row>
-    <row r="26" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D26" s="9">
-        <v>2738</v>
+        <v>2824</v>
       </c>
       <c r="E26" s="9">
         <v>0</v>
       </c>
       <c r="F26" s="9">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)+_xlfn.XLOOKUP("Extra size", $1:$1, 26:26)</f>
+        <v>2824</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2</v>
+      </c>
+      <c r="J26" s="4">
+        <v>2</v>
+      </c>
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4">
+        <v>2</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2</v>
+      </c>
+      <c r="P26" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0</v>
+      </c>
+      <c r="R26" s="4">
+        <v>2</v>
+      </c>
+      <c r="S26" s="4">
+        <v>2</v>
+      </c>
+      <c r="T26" s="4">
+        <v>0</v>
+      </c>
+      <c r="U26" s="4">
+        <v>0</v>
+      </c>
+      <c r="V26" s="4">
+        <v>0</v>
+      </c>
+      <c r="W26" s="4">
+        <v>2</v>
+      </c>
+      <c r="X26" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG26" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH26" s="6">
+        <f>COUNTIF($G26:$BG26, "&gt;0")</f>
+        <v>18</v>
+      </c>
+      <c r="BI26" s="10">
+        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)/_xlfn.XLOOKUP("Feature count", $1:$1, 26:26)</f>
+        <v>156.88888888888889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="9">
         <v>2738</v>
-      </c>
-      <c r="G26" s="4">
-        <v>2</v>
-      </c>
-      <c r="H26" s="4">
-        <v>2</v>
-      </c>
-      <c r="I26" s="4">
-        <v>2</v>
-      </c>
-      <c r="J26" s="4">
-        <v>2</v>
-      </c>
-      <c r="K26" s="4">
-        <v>2</v>
-      </c>
-      <c r="L26" s="4">
-        <v>2</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0</v>
-      </c>
-      <c r="N26" s="4">
-        <v>2</v>
-      </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
-      <c r="P26" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>2</v>
-      </c>
-      <c r="R26" s="4">
-        <v>2</v>
-      </c>
-      <c r="S26" s="4">
-        <v>0</v>
-      </c>
-      <c r="T26" s="4">
-        <v>0</v>
-      </c>
-      <c r="U26" s="4">
-        <v>2</v>
-      </c>
-      <c r="V26" s="4">
-        <v>0</v>
-      </c>
-      <c r="W26" s="4">
-        <v>0</v>
-      </c>
-      <c r="X26" s="4">
-        <v>2</v>
-      </c>
-      <c r="Y26" s="4">
-        <v>2</v>
-      </c>
-      <c r="Z26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="4">
-        <v>2</v>
-      </c>
-      <c r="AB26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE26" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF26" s="4">
-        <v>2</v>
-      </c>
-      <c r="AG26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="4">
-        <v>2</v>
-      </c>
-      <c r="AI26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY26" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BC26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BE26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BF26" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG26" s="6">
-        <f>COUNTIF($G26:$BF26, "&gt;0")</f>
-        <v>17</v>
-      </c>
-      <c r="BH26" s="10">
-        <f>_xlfn.XLOOKUP("Main size", $1:$1, 26:26)/_xlfn.XLOOKUP("Feature count", $1:$1, 26:26)</f>
-        <v>161.05882352941177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="9">
-        <v>2824</v>
       </c>
       <c r="E27" s="9">
         <v>0</v>
       </c>
       <c r="F27" s="9">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)+_xlfn.XLOOKUP("Extra size", $1:$1, 27:27)</f>
-        <v>2824</v>
+        <v>2738</v>
       </c>
       <c r="G27" s="4">
         <v>2</v>
@@ -5733,43 +5816,43 @@
         <v>2</v>
       </c>
       <c r="O27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R27" s="4">
         <v>2</v>
       </c>
       <c r="S27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T27" s="4">
         <v>0</v>
       </c>
       <c r="U27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V27" s="4">
         <v>0</v>
       </c>
       <c r="W27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y27" s="4">
         <v>2</v>
       </c>
       <c r="Z27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB27" s="4">
         <v>0</v>
@@ -5781,16 +5864,16 @@
         <v>2</v>
       </c>
       <c r="AE27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF27" s="4">
         <v>2</v>
       </c>
       <c r="AG27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI27" s="4">
         <v>0</v>
@@ -5864,16 +5947,19 @@
       <c r="BF27" s="4">
         <v>0</v>
       </c>
-      <c r="BG27" s="6">
-        <f>COUNTIF($G27:$BF27, "&gt;0")</f>
+      <c r="BG27" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH27" s="6">
+        <f>COUNTIF($G27:$BG27, "&gt;0")</f>
         <v>17</v>
       </c>
-      <c r="BH27" s="10">
+      <c r="BI27" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 27:27)/_xlfn.XLOOKUP("Feature count", $1:$1, 27:27)</f>
-        <v>166.11764705882354</v>
+        <v>161.05882352941177</v>
       </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>103</v>
       </c>
@@ -6049,16 +6135,19 @@
       <c r="BF28" s="4">
         <v>0</v>
       </c>
-      <c r="BG28" s="6">
-        <f>COUNTIF($G28:$BF28, "&gt;0")</f>
+      <c r="BG28" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH28" s="6">
+        <f>COUNTIF($G28:$BG28, "&gt;0")</f>
         <v>16</v>
       </c>
-      <c r="BH28" s="10">
+      <c r="BI28" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 28:28)/_xlfn.XLOOKUP("Feature count", $1:$1, 28:28)</f>
         <v>169.375</v>
       </c>
     </row>
-    <row r="29" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>102</v>
       </c>
@@ -6234,16 +6323,19 @@
       <c r="BF29" s="4">
         <v>0</v>
       </c>
-      <c r="BG29" s="6">
-        <f>COUNTIF($G29:$BF29, "&gt;0")</f>
+      <c r="BG29" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH29" s="6">
+        <f>COUNTIF($G29:$BG29, "&gt;0")</f>
         <v>17</v>
       </c>
-      <c r="BH29" s="10">
+      <c r="BI29" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 29:29)/_xlfn.XLOOKUP("Feature count", $1:$1, 29:29)</f>
         <v>169.52941176470588</v>
       </c>
     </row>
-    <row r="30" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>104</v>
       </c>
@@ -6393,19 +6485,19 @@
         <v>0</v>
       </c>
       <c r="AX30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY30" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ30" s="4">
         <v>0</v>
       </c>
       <c r="BA30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB30" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC30" s="4">
         <v>0</v>
@@ -6414,21 +6506,24 @@
         <v>0</v>
       </c>
       <c r="BE30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF30" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG30" s="6">
-        <f>COUNTIF($G30:$BF30, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="BG30" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH30" s="6">
+        <f>COUNTIF($G30:$BG30, "&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="BH30" s="10">
+      <c r="BI30" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 30:30)/_xlfn.XLOOKUP("Feature count", $1:$1, 30:30)</f>
         <v>178.04347826086956</v>
       </c>
     </row>
-    <row r="31" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>105</v>
       </c>
@@ -6539,7 +6634,7 @@
         <v>0</v>
       </c>
       <c r="AK31" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL31" s="4">
         <v>0</v>
@@ -6560,10 +6655,10 @@
         <v>0</v>
       </c>
       <c r="AR31" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS31" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT31" s="4">
         <v>0</v>
@@ -6602,21 +6697,24 @@
         <v>0</v>
       </c>
       <c r="BF31" s="4">
-        <v>2</v>
-      </c>
-      <c r="BG31" s="6">
-        <f>COUNTIF($G31:$BF31, "&gt;0")</f>
-        <v>21</v>
-      </c>
-      <c r="BH31" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="4">
+        <v>2</v>
+      </c>
+      <c r="BH31" s="6">
+        <f>COUNTIF($G31:$BG31, "&gt;0")</f>
+        <v>22</v>
+      </c>
+      <c r="BI31" s="10">
         <f>_xlfn.XLOOKUP("Main size", $1:$1, 31:31)/_xlfn.XLOOKUP("Feature count", $1:$1, 31:31)</f>
-        <v>190.57142857142858</v>
+        <v>181.90909090909091</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:BH31" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:BH31">
-      <sortCondition ref="BH3:BH31"/>
+  <autoFilter ref="A3:BI31" xr:uid="{8512C64C-DE47-334B-AE0C-39DDD4F96E15}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:BI31">
+      <sortCondition ref="BI3:BI31"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6655,7 +6753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:BF31">
+  <conditionalFormatting sqref="G4:BG31">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -6666,7 +6764,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG4:BG31">
+  <conditionalFormatting sqref="BH4:BH31">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -6676,7 +6774,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH4:BH31">
+  <conditionalFormatting sqref="BI4:BI31">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -6692,8 +6790,8 @@
     <hyperlink ref="A24" r:id="rId3" xr:uid="{A76D4E5E-9C61-C846-BF68-39EA20E19271}"/>
     <hyperlink ref="A28" r:id="rId4" xr:uid="{271A3F43-6A28-9044-9B77-55CB67E8E604}"/>
     <hyperlink ref="A29" r:id="rId5" xr:uid="{3319FE9B-1572-7B45-A51A-8631F49908F5}"/>
-    <hyperlink ref="A26" r:id="rId6" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
-    <hyperlink ref="A27" r:id="rId7" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
+    <hyperlink ref="A27" r:id="rId6" xr:uid="{6A5AEB05-49D4-5A43-AC85-14DC910FF378}"/>
+    <hyperlink ref="A26" r:id="rId7" xr:uid="{692BC8D6-C410-5A4C-9AC4-692F65427B7C}"/>
     <hyperlink ref="A21" r:id="rId8" xr:uid="{7A0C5CE4-FDBB-C142-89E0-609051079143}"/>
     <hyperlink ref="A25" r:id="rId9" xr:uid="{B27A7A0A-1947-624B-A135-AC2E4FA9DCDF}"/>
     <hyperlink ref="A18" r:id="rId10" xr:uid="{BBFDB1C2-F4D5-9F4F-9AB4-84F69F8E341F}"/>
@@ -6702,8 +6800,8 @@
     <hyperlink ref="A22" r:id="rId13" xr:uid="{1A073B5B-BE69-9E43-BB31-2AC1F74931C7}"/>
     <hyperlink ref="A17" r:id="rId14" xr:uid="{65802411-1B8E-064F-A6D7-DAD404DC6F66}"/>
     <hyperlink ref="A15" r:id="rId15" xr:uid="{8DAB0B02-5401-BF46-90F9-B2B728905C99}"/>
-    <hyperlink ref="A13" r:id="rId16" xr:uid="{F2854865-7589-3148-9BD0-694117F0C02A}"/>
-    <hyperlink ref="A14" r:id="rId17" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
+    <hyperlink ref="A14" r:id="rId16" xr:uid="{F2854865-7589-3148-9BD0-694117F0C02A}"/>
+    <hyperlink ref="A13" r:id="rId17" xr:uid="{0305B1A2-7666-264C-831F-82265021FFB7}"/>
     <hyperlink ref="A12" r:id="rId18" xr:uid="{2F1BE129-94F7-DB45-B74A-D5DECFC8BD1F}"/>
     <hyperlink ref="A11" r:id="rId19" xr:uid="{022DC04F-D95A-7246-8451-7C3BA522CD1C}"/>
     <hyperlink ref="A9" r:id="rId20" xr:uid="{0C291FB0-BA8C-E141-98A4-91A6B6DD9884}"/>

</xml_diff>